<commit_message>
Updated BOM and fixed all ERC and DRC errors
</commit_message>
<xml_diff>
--- a/PCB/Output/BOM.xlsx
+++ b/PCB/Output/BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
   <si>
     <t xml:space="preserve">Number of Boards</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>C201,C301,C303,C304,C305,C306,C307,C401,C402,C403,C404,C405</t>
+    <t>C201,C301,C303,C304,C305,C306,C307,C401,C402,C403,C404,C405,C601</t>
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/yageo/CC0603KRX7R7BB104/302822</t>
@@ -174,19 +174,7 @@
     <t>CON-SMA-EDGE-S-ND</t>
   </si>
   <si>
-    <t>Q701,Q702,Q703</t>
-  </si>
-  <si>
-    <t>MMBT3904</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/diotec-semiconductor/MMBT3904/13163698</t>
-  </si>
-  <si>
-    <t>4878-MMBT3904CT-ND</t>
-  </si>
-  <si>
-    <t>R201,R202,R701,R708,R713</t>
+    <t>R201,R202,R701,R705,R708,R713</t>
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0603FT1K00/1761077</t>
@@ -195,7 +183,7 @@
     <t>RMCF0603FT1K00CT-ND</t>
   </si>
   <si>
-    <t>R301,R302,R401,R402,R707,R712,R717</t>
+    <t>R301,R302,R401,R402,R702,R703,R707,R709,R712,R714,R717</t>
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0603JT10K0/1758104</t>
@@ -204,7 +192,7 @@
     <t>RMCF0603JT10K0CT-ND</t>
   </si>
   <si>
-    <t>R501,R502</t>
+    <t>R303,R304,R501,R502,R718,R720,R722</t>
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/yageo/RC0603FR-075K1L/727268</t>
@@ -213,9 +201,6 @@
     <t>311-5.10KHRCT-ND</t>
   </si>
   <si>
-    <t>R702,R703,R709,R714</t>
-  </si>
-  <si>
     <t>R704,R710,R715</t>
   </si>
   <si>
@@ -225,7 +210,7 @@
     <t>13-RT0603BRD07500RLCT-ND</t>
   </si>
   <si>
-    <t>R705,R706,R711,R716</t>
+    <t>R706,R711,R716,R719,R721,R723</t>
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/panasonic-electronic-components/ERA-3AEB302V/1465865</t>
@@ -370,6 +355,12 @@
   </si>
   <si>
     <t xml:space="preserve">Parts per Board</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Require Parts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extra Parts</t>
   </si>
 </sst>
 </file>
@@ -384,12 +375,12 @@
     <numFmt numFmtId="168" formatCode="000.0\p"/>
     <numFmt numFmtId="169" formatCode="00.0\n"/>
     <numFmt numFmtId="170" formatCode="00.0\p\F"/>
-    <numFmt numFmtId="171" formatCode="0.0\p"/>
-    <numFmt numFmtId="172" formatCode="0.0\k"/>
-    <numFmt numFmtId="173" formatCode="000.0\n"/>
-    <numFmt numFmtId="174" formatCode="00.0\k"/>
-    <numFmt numFmtId="175" formatCode="0.00\p"/>
-    <numFmt numFmtId="176" formatCode="0.00\k"/>
+    <numFmt numFmtId="171" formatCode="0.0\k"/>
+    <numFmt numFmtId="172" formatCode="0.0\p"/>
+    <numFmt numFmtId="173" formatCode="00.0\k"/>
+    <numFmt numFmtId="174" formatCode="000.0\n"/>
+    <numFmt numFmtId="175" formatCode="0.00\k"/>
+    <numFmt numFmtId="176" formatCode="0.00\p"/>
     <numFmt numFmtId="177" formatCode="000.0\m\A"/>
     <numFmt numFmtId="178" formatCode="0.00\n"/>
     <numFmt numFmtId="179" formatCode="00.0\u"/>
@@ -409,12 +400,15 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="none"/>
@@ -429,11 +423,12 @@
       <diagonal style="none"/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="44" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -464,11 +459,20 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="178" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="179" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="9" xfId="2" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="180" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -937,7 +941,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="Z1" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1078,6 +1082,9 @@
         <v>17</v>
       </c>
       <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="4"/>
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
       <c r="AC3" s="2"/>
@@ -1133,6 +1140,9 @@
       <c r="L4" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="4"/>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
       <c r="AC4" s="2"/>
@@ -1184,6 +1194,9 @@
       <c r="L5" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="8"/>
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
@@ -1235,6 +1248,9 @@
       <c r="L6" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
@@ -1284,6 +1300,9 @@
       <c r="L7" t="s">
         <v>31</v>
       </c>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
@@ -1337,6 +1356,9 @@
       <c r="L8" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
@@ -1392,6 +1414,9 @@
       <c r="L9" t="s">
         <v>39</v>
       </c>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
@@ -1447,6 +1472,9 @@
       <c r="L10" t="s">
         <v>43</v>
       </c>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
@@ -1502,6 +1530,9 @@
       <c r="L11" t="s">
         <v>47</v>
       </c>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
@@ -1557,6 +1588,9 @@
       <c r="L12" s="2" t="s">
         <v>51</v>
       </c>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
       <c r="AC12" s="2"/>
@@ -1577,45 +1611,48 @@
         <v>52</v>
       </c>
       <c r="B13" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C13" s="7">
         <f>$C$1*B13</f>
-        <v>3</v>
-      </c>
-      <c r="D13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13">
-        <v>0.11</v>
-      </c>
-      <c r="G13">
-        <v>0.065000000000000002</v>
-      </c>
-      <c r="H13">
-        <v>0.039800000000000002</v>
-      </c>
-      <c r="I13">
-        <v>0.024969999999999999</v>
+      <c r="F13" s="2">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0.0091000000000000004</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0.0047999999999999996</v>
       </c>
       <c r="J13" s="6">
         <f>IF(MIN(IF(I13=0,1000000,I13*ROUNDUP(C13,-3)),IF(H13=0,1000000,H13*ROUNDUP(C13,-2)),IF(G13=0,1000000,G13*ROUNDUP(C13,-1)),IF(F13=0,1000000,F13*C13))=1000000,0,MIN(IF(I13=0,1000000,I13*ROUNDUP(C13,-3)),IF(H13=0,1000000,H13*ROUNDUP(C13,-2)),IF(G13=0,1000000,G13*ROUNDUP(C13,-1)),IF(F13=0,1000000,F13*C13)))</f>
-        <v>0.33000000000000002</v>
+        <v>0.20000000000000001</v>
       </c>
       <c r="K13" s="2">
         <f>IF(J13=IF(F13=0,1000000,F13*C13),C13,IF(J13=IF(G13=0,1000000,G13*ROUNDUP(C13,-1)),ROUNDUP(C13,-1),IF(J13=IF(H13=0,1000000,H13*ROUNDUP(C13,-2)),ROUNDUP(C13,-2),IF(J13=IF(I13=0,1000000,I13*ROUNDUP(C13,-3)),ROUNDUP(C13,-3),0))))</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="L13" t="s">
-        <v>55</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="13"/>
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
       <c r="AC13" s="2"/>
-      <c r="AD13" s="13"/>
+      <c r="AD13" s="14"/>
       <c r="AE13" s="5"/>
       <c r="AF13" s="2"/>
       <c r="AG13" s="2"/>
@@ -1629,48 +1666,51 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" s="2">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C14" s="7">
         <f>$C$1*B14</f>
-        <v>5</v>
-      </c>
-      <c r="D14" s="14">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="D14" s="15">
+        <v>10</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F14" s="2">
         <v>0.10000000000000001</v>
       </c>
       <c r="G14" s="2">
-        <v>0.02</v>
+        <v>0.019</v>
       </c>
       <c r="H14" s="2">
-        <v>0.0091000000000000004</v>
+        <v>0.0086</v>
       </c>
       <c r="I14" s="2">
-        <v>0.0047999999999999996</v>
+        <v>0.0044799999999999996</v>
       </c>
       <c r="J14" s="6">
         <f>IF(MIN(IF(I14=0,1000000,I14*ROUNDUP(C14,-3)),IF(H14=0,1000000,H14*ROUNDUP(C14,-2)),IF(G14=0,1000000,G14*ROUNDUP(C14,-1)),IF(F14=0,1000000,F14*C14))=1000000,0,MIN(IF(I14=0,1000000,I14*ROUNDUP(C14,-3)),IF(H14=0,1000000,H14*ROUNDUP(C14,-2)),IF(G14=0,1000000,G14*ROUNDUP(C14,-1)),IF(F14=0,1000000,F14*C14)))</f>
-        <v>0.20000000000000001</v>
+        <v>0.38</v>
       </c>
       <c r="K14" s="2">
         <f>IF(J14=IF(F14=0,1000000,F14*C14),C14,IF(J14=IF(G14=0,1000000,G14*ROUNDUP(C14,-1)),ROUNDUP(C14,-1),IF(J14=IF(H14=0,1000000,H14*ROUNDUP(C14,-2)),ROUNDUP(C14,-2),IF(J14=IF(I14=0,1000000,I14*ROUNDUP(C14,-3)),ROUNDUP(C14,-3),0))))</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L14" t="s">
-        <v>58</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="15"/>
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
       <c r="AC14" s="2"/>
-      <c r="AD14" s="15"/>
+      <c r="AD14" s="16"/>
       <c r="AE14" s="5"/>
       <c r="AF14" s="2"/>
       <c r="AG14" s="2"/>
@@ -1684,7 +1724,7 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" s="2">
         <v>7</v>
@@ -1693,39 +1733,42 @@
         <f>$C$1*B15</f>
         <v>7</v>
       </c>
-      <c r="D15" s="16">
-        <v>10</v>
+      <c r="D15" s="17">
+        <v>5.0999999999999996</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F15" s="2">
         <v>0.10000000000000001</v>
       </c>
       <c r="G15" s="2">
-        <v>0.019</v>
+        <v>0.089999999999999997</v>
       </c>
       <c r="H15" s="2">
-        <v>0.0086</v>
+        <v>0.0082000000000000007</v>
       </c>
       <c r="I15" s="2">
-        <v>0.0044799999999999996</v>
+        <v>0.0051000000000000004</v>
       </c>
       <c r="J15" s="6">
         <f>IF(MIN(IF(I15=0,1000000,I15*ROUNDUP(C15,-3)),IF(H15=0,1000000,H15*ROUNDUP(C15,-2)),IF(G15=0,1000000,G15*ROUNDUP(C15,-1)),IF(F15=0,1000000,F15*C15))=1000000,0,MIN(IF(I15=0,1000000,I15*ROUNDUP(C15,-3)),IF(H15=0,1000000,H15*ROUNDUP(C15,-2)),IF(G15=0,1000000,G15*ROUNDUP(C15,-1)),IF(F15=0,1000000,F15*C15)))</f>
-        <v>0.19</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="K15" s="2">
         <f>IF(J15=IF(F15=0,1000000,F15*C15),C15,IF(J15=IF(G15=0,1000000,G15*ROUNDUP(C15,-1)),ROUNDUP(C15,-1),IF(J15=IF(H15=0,1000000,H15*ROUNDUP(C15,-2)),ROUNDUP(C15,-2),IF(J15=IF(I15=0,1000000,I15*ROUNDUP(C15,-3)),ROUNDUP(C15,-3),0))))</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L15" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="17"/>
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
-      <c r="AD15" s="17"/>
+      <c r="AD15" s="18"/>
       <c r="AE15" s="5"/>
       <c r="AF15" s="2"/>
       <c r="AG15" s="2"/>
@@ -1739,48 +1782,51 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B16" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C16" s="7">
         <f>$C$1*B16</f>
-        <v>4</v>
-      </c>
-      <c r="D16" s="18">
-        <v>5.0999999999999996</v>
+        <v>3</v>
+      </c>
+      <c r="D16" s="2">
+        <v>500</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F16" s="2">
         <v>0.10000000000000001</v>
       </c>
       <c r="G16" s="2">
-        <v>0.089999999999999997</v>
+        <v>0.064000000000000001</v>
       </c>
       <c r="H16" s="2">
-        <v>0.0082000000000000007</v>
+        <v>0.0533</v>
       </c>
       <c r="I16" s="2">
-        <v>0.0051000000000000004</v>
+        <v>0.044319999999999998</v>
       </c>
       <c r="J16" s="6">
         <f>IF(MIN(IF(I16=0,1000000,I16*ROUNDUP(C16,-3)),IF(H16=0,1000000,H16*ROUNDUP(C16,-2)),IF(G16=0,1000000,G16*ROUNDUP(C16,-1)),IF(F16=0,1000000,F16*C16))=1000000,0,MIN(IF(I16=0,1000000,I16*ROUNDUP(C16,-3)),IF(H16=0,1000000,H16*ROUNDUP(C16,-2)),IF(G16=0,1000000,G16*ROUNDUP(C16,-1)),IF(F16=0,1000000,F16*C16)))</f>
-        <v>0.40000000000000002</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="K16" s="2">
         <f>IF(J16=IF(F16=0,1000000,F16*C16),C16,IF(J16=IF(G16=0,1000000,G16*ROUNDUP(C16,-1)),ROUNDUP(C16,-1),IF(J16=IF(H16=0,1000000,H16*ROUNDUP(C16,-2)),ROUNDUP(C16,-2),IF(J16=IF(I16=0,1000000,I16*ROUNDUP(C16,-3)),ROUNDUP(C16,-3),0))))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L16" t="s">
-        <v>64</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
       <c r="AA16" s="2"/>
       <c r="AB16" s="2"/>
       <c r="AC16" s="2"/>
-      <c r="AD16" s="17"/>
+      <c r="AD16" s="18"/>
       <c r="AE16" s="5"/>
       <c r="AF16" s="2"/>
       <c r="AG16" s="2"/>
@@ -1794,48 +1840,51 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B17" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C17" s="7">
         <f>$C$1*B17</f>
-        <v>4</v>
-      </c>
-      <c r="D17" s="16">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="D17" s="13">
+        <v>3</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="F17" s="2">
         <v>0.10000000000000001</v>
       </c>
       <c r="G17" s="2">
-        <v>0.019</v>
+        <v>0.060999999999999999</v>
       </c>
       <c r="H17" s="2">
-        <v>0.0086</v>
+        <v>0.050599999999999999</v>
       </c>
       <c r="I17" s="2">
-        <v>0.0044799999999999996</v>
+        <v>0.04206</v>
       </c>
       <c r="J17" s="6">
         <f>IF(MIN(IF(I17=0,1000000,I17*ROUNDUP(C17,-3)),IF(H17=0,1000000,H17*ROUNDUP(C17,-2)),IF(G17=0,1000000,G17*ROUNDUP(C17,-1)),IF(F17=0,1000000,F17*C17))=1000000,0,MIN(IF(I17=0,1000000,I17*ROUNDUP(C17,-3)),IF(H17=0,1000000,H17*ROUNDUP(C17,-2)),IF(G17=0,1000000,G17*ROUNDUP(C17,-1)),IF(F17=0,1000000,F17*C17)))</f>
-        <v>0.19</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="K17" s="2">
         <f>IF(J17=IF(F17=0,1000000,F17*C17),C17,IF(J17=IF(G17=0,1000000,G17*ROUNDUP(C17,-1)),ROUNDUP(C17,-1),IF(J17=IF(H17=0,1000000,H17*ROUNDUP(C17,-2)),ROUNDUP(C17,-2),IF(J17=IF(I17=0,1000000,I17*ROUNDUP(C17,-3)),ROUNDUP(C17,-3),0))))</f>
-        <v>10</v>
-      </c>
-      <c r="L17" t="s">
-        <v>61</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="L17" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="13"/>
       <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
       <c r="AC17" s="2"/>
-      <c r="AD17" s="13"/>
+      <c r="AD17" s="14"/>
       <c r="AE17" s="5"/>
       <c r="AF17" s="2"/>
       <c r="AG17" s="2"/>
@@ -1849,44 +1898,47 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B18" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C18" s="7">
         <f>$C$1*B18</f>
-        <v>3</v>
-      </c>
-      <c r="D18" s="2">
-        <v>500</v>
+        <v>1</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F18" s="2">
-        <v>0.10000000000000001</v>
+        <v>1.3799999999999999</v>
       </c>
       <c r="G18" s="2">
-        <v>0.064000000000000001</v>
+        <v>1.0069999999999999</v>
       </c>
       <c r="H18" s="2">
-        <v>0.0533</v>
+        <v>0.80930000000000002</v>
       </c>
       <c r="I18" s="2">
-        <v>0.044319999999999998</v>
+        <v>0.70565</v>
       </c>
       <c r="J18" s="6">
         <f>IF(MIN(IF(I18=0,1000000,I18*ROUNDUP(C18,-3)),IF(H18=0,1000000,H18*ROUNDUP(C18,-2)),IF(G18=0,1000000,G18*ROUNDUP(C18,-1)),IF(F18=0,1000000,F18*C18))=1000000,0,MIN(IF(I18=0,1000000,I18*ROUNDUP(C18,-3)),IF(H18=0,1000000,H18*ROUNDUP(C18,-2)),IF(G18=0,1000000,G18*ROUNDUP(C18,-1)),IF(F18=0,1000000,F18*C18)))</f>
-        <v>0.30000000000000004</v>
+        <v>1.3799999999999999</v>
       </c>
       <c r="K18" s="2">
         <f>IF(J18=IF(F18=0,1000000,F18*C18),C18,IF(J18=IF(G18=0,1000000,G18*ROUNDUP(C18,-1)),ROUNDUP(C18,-1),IF(J18=IF(H18=0,1000000,H18*ROUNDUP(C18,-2)),ROUNDUP(C18,-2),IF(J18=IF(I18=0,1000000,I18*ROUNDUP(C18,-3)),ROUNDUP(C18,-3),0))))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L18" t="s">
-        <v>68</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
       <c r="AA18" s="2"/>
       <c r="AB18" s="2"/>
       <c r="AC18" s="2"/>
@@ -1904,44 +1956,47 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B19" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C19" s="7">
         <f>$C$1*B19</f>
-        <v>4</v>
-      </c>
-      <c r="D19" s="14">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F19" s="2">
-        <v>0.10000000000000001</v>
+        <v>1.53</v>
       </c>
       <c r="G19" s="2">
-        <v>0.060999999999999999</v>
+        <v>1.431</v>
       </c>
       <c r="H19" s="2">
-        <v>0.050599999999999999</v>
+        <v>1.3285</v>
       </c>
       <c r="I19" s="2">
-        <v>0.04206</v>
+        <v>1.2256800000000001</v>
       </c>
       <c r="J19" s="6">
         <f>IF(MIN(IF(I19=0,1000000,I19*ROUNDUP(C19,-3)),IF(H19=0,1000000,H19*ROUNDUP(C19,-2)),IF(G19=0,1000000,G19*ROUNDUP(C19,-1)),IF(F19=0,1000000,F19*C19))=1000000,0,MIN(IF(I19=0,1000000,I19*ROUNDUP(C19,-3)),IF(H19=0,1000000,H19*ROUNDUP(C19,-2)),IF(G19=0,1000000,G19*ROUNDUP(C19,-1)),IF(F19=0,1000000,F19*C19)))</f>
-        <v>0.40000000000000002</v>
+        <v>1.53</v>
       </c>
       <c r="K19" s="2">
         <f>IF(J19=IF(F19=0,1000000,F19*C19),C19,IF(J19=IF(G19=0,1000000,G19*ROUNDUP(C19,-1)),ROUNDUP(C19,-1),IF(J19=IF(H19=0,1000000,H19*ROUNDUP(C19,-2)),ROUNDUP(C19,-2),IF(J19=IF(I19=0,1000000,I19*ROUNDUP(C19,-3)),ROUNDUP(C19,-3),0))))</f>
-        <v>4</v>
-      </c>
-      <c r="L19" s="19" t="s">
-        <v>71</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="L19" t="s">
+        <v>74</v>
+      </c>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
       <c r="AA19" s="2"/>
       <c r="AB19" s="2"/>
       <c r="AC19" s="2"/>
@@ -1959,7 +2014,7 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B20" s="2">
         <v>1</v>
@@ -1969,34 +2024,33 @@
         <v>1</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F20" s="2">
-        <v>1.3799999999999999</v>
+        <v>8.6099999999999994</v>
       </c>
       <c r="G20" s="2">
-        <v>1.0069999999999999</v>
-      </c>
-      <c r="H20" s="2">
-        <v>0.80930000000000002</v>
-      </c>
-      <c r="I20" s="2">
-        <v>0.70565</v>
-      </c>
+        <v>6.6849999999999996</v>
+      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
       <c r="J20" s="6">
         <f>IF(MIN(IF(I20=0,1000000,I20*ROUNDUP(C20,-3)),IF(H20=0,1000000,H20*ROUNDUP(C20,-2)),IF(G20=0,1000000,G20*ROUNDUP(C20,-1)),IF(F20=0,1000000,F20*C20))=1000000,0,MIN(IF(I20=0,1000000,I20*ROUNDUP(C20,-3)),IF(H20=0,1000000,H20*ROUNDUP(C20,-2)),IF(G20=0,1000000,G20*ROUNDUP(C20,-1)),IF(F20=0,1000000,F20*C20)))</f>
-        <v>1.3799999999999999</v>
+        <v>8.6099999999999994</v>
       </c>
       <c r="K20" s="2">
         <f>IF(J20=IF(F20=0,1000000,F20*C20),C20,IF(J20=IF(G20=0,1000000,G20*ROUNDUP(C20,-1)),ROUNDUP(C20,-1),IF(J20=IF(H20=0,1000000,H20*ROUNDUP(C20,-2)),ROUNDUP(C20,-2),IF(J20=IF(I20=0,1000000,I20*ROUNDUP(C20,-3)),ROUNDUP(C20,-3),0))))</f>
         <v>1</v>
       </c>
       <c r="L20" t="s">
-        <v>75</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
       <c r="AA20" s="2"/>
       <c r="AB20" s="2"/>
       <c r="AC20" s="2"/>
@@ -2014,7 +2068,7 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B21" s="2">
         <v>1</v>
@@ -2024,34 +2078,37 @@
         <v>1</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F21" s="2">
-        <v>1.53</v>
+        <v>0.95999999999999996</v>
       </c>
       <c r="G21" s="2">
-        <v>1.431</v>
+        <v>0.81000000000000005</v>
       </c>
       <c r="H21" s="2">
-        <v>1.3285</v>
+        <v>0.68359999999999999</v>
       </c>
       <c r="I21" s="2">
-        <v>1.2256800000000001</v>
+        <v>0.59601000000000004</v>
       </c>
       <c r="J21" s="6">
         <f>IF(MIN(IF(I21=0,1000000,I21*ROUNDUP(C21,-3)),IF(H21=0,1000000,H21*ROUNDUP(C21,-2)),IF(G21=0,1000000,G21*ROUNDUP(C21,-1)),IF(F21=0,1000000,F21*C21))=1000000,0,MIN(IF(I21=0,1000000,I21*ROUNDUP(C21,-3)),IF(H21=0,1000000,H21*ROUNDUP(C21,-2)),IF(G21=0,1000000,G21*ROUNDUP(C21,-1)),IF(F21=0,1000000,F21*C21)))</f>
-        <v>1.53</v>
+        <v>0.95999999999999996</v>
       </c>
       <c r="K21" s="2">
         <f>IF(J21=IF(F21=0,1000000,F21*C21),C21,IF(J21=IF(G21=0,1000000,G21*ROUNDUP(C21,-1)),ROUNDUP(C21,-1),IF(J21=IF(H21=0,1000000,H21*ROUNDUP(C21,-2)),ROUNDUP(C21,-2),IF(J21=IF(I21=0,1000000,I21*ROUNDUP(C21,-3)),ROUNDUP(C21,-3),0))))</f>
         <v>1</v>
       </c>
       <c r="L21" t="s">
-        <v>79</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
       <c r="AA21" s="2"/>
       <c r="AB21" s="2"/>
       <c r="AC21" s="2"/>
@@ -2069,7 +2126,7 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B22" s="2">
         <v>1</v>
@@ -2079,30 +2136,37 @@
         <v>1</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F22" s="2">
-        <v>8.6099999999999994</v>
+        <v>7.2599999999999998</v>
       </c>
       <c r="G22" s="2">
-        <v>6.6849999999999996</v>
-      </c>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
+        <v>6.282</v>
+      </c>
+      <c r="H22" s="2">
+        <v>5.9656000000000002</v>
+      </c>
+      <c r="I22" s="2">
+        <v>5.5507999999999997</v>
+      </c>
       <c r="J22" s="6">
         <f>IF(MIN(IF(I22=0,1000000,I22*ROUNDUP(C22,-3)),IF(H22=0,1000000,H22*ROUNDUP(C22,-2)),IF(G22=0,1000000,G22*ROUNDUP(C22,-1)),IF(F22=0,1000000,F22*C22))=1000000,0,MIN(IF(I22=0,1000000,I22*ROUNDUP(C22,-3)),IF(H22=0,1000000,H22*ROUNDUP(C22,-2)),IF(G22=0,1000000,G22*ROUNDUP(C22,-1)),IF(F22=0,1000000,F22*C22)))</f>
-        <v>8.6099999999999994</v>
+        <v>7.2599999999999998</v>
       </c>
       <c r="K22" s="2">
         <f>IF(J22=IF(F22=0,1000000,F22*C22),C22,IF(J22=IF(G22=0,1000000,G22*ROUNDUP(C22,-1)),ROUNDUP(C22,-1),IF(J22=IF(H22=0,1000000,H22*ROUNDUP(C22,-2)),ROUNDUP(C22,-2),IF(J22=IF(I22=0,1000000,I22*ROUNDUP(C22,-3)),ROUNDUP(C22,-3),0))))</f>
         <v>1</v>
       </c>
       <c r="L22" t="s">
-        <v>83</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
       <c r="AA22" s="2"/>
       <c r="AB22" s="2"/>
       <c r="AC22" s="2"/>
@@ -2120,7 +2184,7 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B23" s="2">
         <v>1</v>
@@ -2130,34 +2194,37 @@
         <v>1</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F23" s="2">
-        <v>0.95999999999999996</v>
+        <v>8.7200000000000006</v>
       </c>
       <c r="G23" s="2">
-        <v>0.81000000000000005</v>
+        <v>7.5700000000000003</v>
       </c>
       <c r="H23" s="2">
-        <v>0.68359999999999999</v>
+        <v>6.7085999999999997</v>
       </c>
       <c r="I23" s="2">
-        <v>0.59601000000000004</v>
+        <v>6.0628700000000002</v>
       </c>
       <c r="J23" s="6">
         <f>IF(MIN(IF(I23=0,1000000,I23*ROUNDUP(C23,-3)),IF(H23=0,1000000,H23*ROUNDUP(C23,-2)),IF(G23=0,1000000,G23*ROUNDUP(C23,-1)),IF(F23=0,1000000,F23*C23))=1000000,0,MIN(IF(I23=0,1000000,I23*ROUNDUP(C23,-3)),IF(H23=0,1000000,H23*ROUNDUP(C23,-2)),IF(G23=0,1000000,G23*ROUNDUP(C23,-1)),IF(F23=0,1000000,F23*C23)))</f>
-        <v>0.95999999999999996</v>
+        <v>8.7200000000000006</v>
       </c>
       <c r="K23" s="2">
         <f>IF(J23=IF(F23=0,1000000,F23*C23),C23,IF(J23=IF(G23=0,1000000,G23*ROUNDUP(C23,-1)),ROUNDUP(C23,-1),IF(J23=IF(H23=0,1000000,H23*ROUNDUP(C23,-2)),ROUNDUP(C23,-2),IF(J23=IF(I23=0,1000000,I23*ROUNDUP(C23,-3)),ROUNDUP(C23,-3),0))))</f>
         <v>1</v>
       </c>
       <c r="L23" t="s">
-        <v>87</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
       <c r="AA23" s="2"/>
       <c r="AB23" s="2"/>
       <c r="AC23" s="2"/>
@@ -2175,7 +2242,7 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B24" s="2">
         <v>1</v>
@@ -2185,34 +2252,35 @@
         <v>1</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="F24" s="2">
-        <v>7.2599999999999998</v>
+        <v>31.5</v>
       </c>
       <c r="G24" s="2">
-        <v>6.282</v>
+        <v>25.91</v>
       </c>
       <c r="H24" s="2">
-        <v>5.9656000000000002</v>
-      </c>
-      <c r="I24" s="2">
-        <v>5.5507999999999997</v>
-      </c>
+        <v>20.853899999999999</v>
+      </c>
+      <c r="I24" s="2"/>
       <c r="J24" s="6">
         <f>IF(MIN(IF(I24=0,1000000,I24*ROUNDUP(C24,-3)),IF(H24=0,1000000,H24*ROUNDUP(C24,-2)),IF(G24=0,1000000,G24*ROUNDUP(C24,-1)),IF(F24=0,1000000,F24*C24))=1000000,0,MIN(IF(I24=0,1000000,I24*ROUNDUP(C24,-3)),IF(H24=0,1000000,H24*ROUNDUP(C24,-2)),IF(G24=0,1000000,G24*ROUNDUP(C24,-1)),IF(F24=0,1000000,F24*C24)))</f>
-        <v>7.2599999999999998</v>
+        <v>31.5</v>
       </c>
       <c r="K24" s="2">
         <f>IF(J24=IF(F24=0,1000000,F24*C24),C24,IF(J24=IF(G24=0,1000000,G24*ROUNDUP(C24,-1)),ROUNDUP(C24,-1),IF(J24=IF(H24=0,1000000,H24*ROUNDUP(C24,-2)),ROUNDUP(C24,-2),IF(J24=IF(I24=0,1000000,I24*ROUNDUP(C24,-3)),ROUNDUP(C24,-3),0))))</f>
         <v>1</v>
       </c>
       <c r="L24" t="s">
-        <v>91</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
       <c r="AA24" s="2"/>
       <c r="AB24" s="2"/>
       <c r="AC24" s="2"/>
@@ -2230,7 +2298,7 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B25" s="2">
         <v>1</v>
@@ -2240,34 +2308,28 @@
         <v>1</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="F25" s="2">
-        <v>8.7200000000000006</v>
-      </c>
-      <c r="G25" s="2">
-        <v>7.5700000000000003</v>
-      </c>
-      <c r="H25" s="2">
-        <v>6.7085999999999997</v>
-      </c>
-      <c r="I25" s="2">
-        <v>6.0628700000000002</v>
+        <v>97</v>
+      </c>
+      <c r="F25">
+        <v>8.1199999999999992</v>
       </c>
       <c r="J25" s="6">
         <f>IF(MIN(IF(I25=0,1000000,I25*ROUNDUP(C25,-3)),IF(H25=0,1000000,H25*ROUNDUP(C25,-2)),IF(G25=0,1000000,G25*ROUNDUP(C25,-1)),IF(F25=0,1000000,F25*C25))=1000000,0,MIN(IF(I25=0,1000000,I25*ROUNDUP(C25,-3)),IF(H25=0,1000000,H25*ROUNDUP(C25,-2)),IF(G25=0,1000000,G25*ROUNDUP(C25,-1)),IF(F25=0,1000000,F25*C25)))</f>
-        <v>8.7200000000000006</v>
+        <v>8.1199999999999992</v>
       </c>
       <c r="K25" s="2">
         <f>IF(J25=IF(F25=0,1000000,F25*C25),C25,IF(J25=IF(G25=0,1000000,G25*ROUNDUP(C25,-1)),ROUNDUP(C25,-1),IF(J25=IF(H25=0,1000000,H25*ROUNDUP(C25,-2)),ROUNDUP(C25,-2),IF(J25=IF(I25=0,1000000,I25*ROUNDUP(C25,-3)),ROUNDUP(C25,-3),0))))</f>
         <v>1</v>
       </c>
       <c r="L25" t="s">
-        <v>95</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
       <c r="AA25" s="2"/>
       <c r="AB25" s="2"/>
       <c r="AC25" s="2"/>
@@ -2285,42 +2347,47 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B26" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C26" s="7">
         <f>$C$1*B26</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="F26" s="2">
-        <v>31.5</v>
+        <v>1.3200000000000001</v>
       </c>
       <c r="G26" s="2">
-        <v>25.91</v>
+        <v>0.85099999999999998</v>
       </c>
       <c r="H26" s="2">
-        <v>20.853899999999999</v>
-      </c>
-      <c r="I26" s="2"/>
+        <v>0.56289999999999996</v>
+      </c>
+      <c r="I26" s="2">
+        <v>0.39964</v>
+      </c>
       <c r="J26" s="6">
         <f>IF(MIN(IF(I26=0,1000000,I26*ROUNDUP(C26,-3)),IF(H26=0,1000000,H26*ROUNDUP(C26,-2)),IF(G26=0,1000000,G26*ROUNDUP(C26,-1)),IF(F26=0,1000000,F26*C26))=1000000,0,MIN(IF(I26=0,1000000,I26*ROUNDUP(C26,-3)),IF(H26=0,1000000,H26*ROUNDUP(C26,-2)),IF(G26=0,1000000,G26*ROUNDUP(C26,-1)),IF(F26=0,1000000,F26*C26)))</f>
-        <v>31.5</v>
+        <v>3.96</v>
       </c>
       <c r="K26" s="2">
         <f>IF(J26=IF(F26=0,1000000,F26*C26),C26,IF(J26=IF(G26=0,1000000,G26*ROUNDUP(C26,-1)),ROUNDUP(C26,-1),IF(J26=IF(H26=0,1000000,H26*ROUNDUP(C26,-2)),ROUNDUP(C26,-2),IF(J26=IF(I26=0,1000000,I26*ROUNDUP(C26,-3)),ROUNDUP(C26,-3),0))))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L26" t="s">
-        <v>99</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
       <c r="AA26" s="2"/>
       <c r="AB26" s="2"/>
       <c r="AC26" s="2"/>
@@ -2338,7 +2405,7 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B27" s="2">
         <v>1</v>
@@ -2348,25 +2415,37 @@
         <v>1</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="F27">
-        <v>8.1199999999999992</v>
+        <v>0.23000000000000001</v>
+      </c>
+      <c r="G27">
+        <v>0.20000000000000001</v>
+      </c>
+      <c r="H27">
+        <v>0.1739</v>
+      </c>
+      <c r="I27">
+        <v>0.15112999999999999</v>
       </c>
       <c r="J27" s="6">
         <f>IF(MIN(IF(I27=0,1000000,I27*ROUNDUP(C27,-3)),IF(H27=0,1000000,H27*ROUNDUP(C27,-2)),IF(G27=0,1000000,G27*ROUNDUP(C27,-1)),IF(F27=0,1000000,F27*C27))=1000000,0,MIN(IF(I27=0,1000000,I27*ROUNDUP(C27,-3)),IF(H27=0,1000000,H27*ROUNDUP(C27,-2)),IF(G27=0,1000000,G27*ROUNDUP(C27,-1)),IF(F27=0,1000000,F27*C27)))</f>
-        <v>8.1199999999999992</v>
+        <v>0.23000000000000001</v>
       </c>
       <c r="K27" s="2">
         <f>IF(J27=IF(F27=0,1000000,F27*C27),C27,IF(J27=IF(G27=0,1000000,G27*ROUNDUP(C27,-1)),ROUNDUP(C27,-1),IF(J27=IF(H27=0,1000000,H27*ROUNDUP(C27,-2)),ROUNDUP(C27,-2),IF(J27=IF(I27=0,1000000,I27*ROUNDUP(C27,-3)),ROUNDUP(C27,-3),0))))</f>
         <v>1</v>
       </c>
       <c r="L27" t="s">
-        <v>103</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
       <c r="AA27" s="2"/>
       <c r="AB27" s="2"/>
       <c r="AC27" s="2"/>
@@ -2384,44 +2463,39 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B28" s="2">
-        <v>3</v>
-      </c>
-      <c r="C28" s="7">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2">
         <f>$C$1*B28</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="F28" s="2">
-        <v>1.3200000000000001</v>
-      </c>
-      <c r="G28" s="2">
-        <v>0.85099999999999998</v>
-      </c>
-      <c r="H28" s="2">
-        <v>0.56289999999999996</v>
-      </c>
-      <c r="I28" s="2">
-        <v>0.39964</v>
-      </c>
+        <f>41.85/3</f>
+        <v>13.950000000000001</v>
+      </c>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
       <c r="J28" s="6">
         <f>IF(MIN(IF(I28=0,1000000,I28*ROUNDUP(C28,-3)),IF(H28=0,1000000,H28*ROUNDUP(C28,-2)),IF(G28=0,1000000,G28*ROUNDUP(C28,-1)),IF(F28=0,1000000,F28*C28))=1000000,0,MIN(IF(I28=0,1000000,I28*ROUNDUP(C28,-3)),IF(H28=0,1000000,H28*ROUNDUP(C28,-2)),IF(G28=0,1000000,G28*ROUNDUP(C28,-1)),IF(F28=0,1000000,F28*C28)))</f>
-        <v>3.96</v>
+        <v>13.950000000000001</v>
       </c>
       <c r="K28" s="2">
         <f>IF(J28=IF(F28=0,1000000,F28*C28),C28,IF(J28=IF(G28=0,1000000,G28*ROUNDUP(C28,-1)),ROUNDUP(C28,-1),IF(J28=IF(H28=0,1000000,H28*ROUNDUP(C28,-2)),ROUNDUP(C28,-2),IF(J28=IF(I28=0,1000000,I28*ROUNDUP(C28,-3)),ROUNDUP(C28,-3),0))))</f>
-        <v>3</v>
-      </c>
-      <c r="L28" t="s">
-        <v>107</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
       <c r="AA28" s="2"/>
       <c r="AB28" s="2"/>
       <c r="AC28" s="2"/>
@@ -2438,49 +2512,13 @@
       <c r="AN28" s="2"/>
     </row>
     <row r="29">
-      <c r="A29" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B29" s="2">
-        <v>1</v>
-      </c>
-      <c r="C29" s="7">
-        <f>$C$1*B29</f>
-        <v>1</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="F29">
-        <v>0.23000000000000001</v>
-      </c>
-      <c r="G29">
-        <v>0.20000000000000001</v>
-      </c>
-      <c r="H29">
-        <v>0.1739</v>
-      </c>
-      <c r="I29">
-        <v>0.15112999999999999</v>
-      </c>
-      <c r="J29" s="6">
-        <f>IF(MIN(IF(I29=0,1000000,I29*ROUNDUP(C29,-3)),IF(H29=0,1000000,H29*ROUNDUP(C29,-2)),IF(G29=0,1000000,G29*ROUNDUP(C29,-1)),IF(F29=0,1000000,F29*C29))=1000000,0,MIN(IF(I29=0,1000000,I29*ROUNDUP(C29,-3)),IF(H29=0,1000000,H29*ROUNDUP(C29,-2)),IF(G29=0,1000000,G29*ROUNDUP(C29,-1)),IF(F29=0,1000000,F29*C29)))</f>
-        <v>0.23000000000000001</v>
-      </c>
-      <c r="K29" s="2">
-        <f>IF(J29=IF(F29=0,1000000,F29*C29),C29,IF(J29=IF(G29=0,1000000,G29*ROUNDUP(C29,-1)),ROUNDUP(C29,-1),IF(J29=IF(H29=0,1000000,H29*ROUNDUP(C29,-2)),ROUNDUP(C29,-2),IF(J29=IF(I29=0,1000000,I29*ROUNDUP(C29,-3)),ROUNDUP(C29,-3),0))))</f>
-        <v>1</v>
-      </c>
-      <c r="L29" t="s">
-        <v>111</v>
-      </c>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
       <c r="AA29" s="2"/>
       <c r="AB29" s="2"/>
       <c r="AC29" s="2"/>
-      <c r="AD29" s="14"/>
+      <c r="AD29" s="13"/>
       <c r="AE29" s="5"/>
       <c r="AF29" s="2"/>
       <c r="AG29" s="2"/>
@@ -2493,34 +2531,9 @@
       <c r="AN29" s="2"/>
     </row>
     <row r="30">
-      <c r="A30" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B30" s="2">
-        <v>1</v>
-      </c>
-      <c r="C30" s="2">
-        <f>$C$1*B30</f>
-        <v>1</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="F30" s="2">
-        <f>41.85/3</f>
-        <v>13.950000000000001</v>
-      </c>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="6">
-        <f>IF(MIN(IF(I30=0,1000000,I30*ROUNDUP(C30,-3)),IF(H30=0,1000000,H30*ROUNDUP(C30,-2)),IF(G30=0,1000000,G30*ROUNDUP(C30,-1)),IF(F30=0,1000000,F30*C30))=1000000,0,MIN(IF(I30=0,1000000,I30*ROUNDUP(C30,-3)),IF(H30=0,1000000,H30*ROUNDUP(C30,-2)),IF(G30=0,1000000,G30*ROUNDUP(C30,-1)),IF(F30=0,1000000,F30*C30)))</f>
-        <v>13.950000000000001</v>
-      </c>
-      <c r="K30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
       <c r="AA30" s="2"/>
       <c r="AB30" s="2"/>
       <c r="AC30" s="2"/>
@@ -2540,7 +2553,7 @@
       <c r="AA31" s="2"/>
       <c r="AB31" s="2"/>
       <c r="AC31" s="2"/>
-      <c r="AD31" s="16"/>
+      <c r="AD31" s="15"/>
       <c r="AE31" s="5"/>
       <c r="AF31" s="2"/>
       <c r="AG31" s="2"/>
@@ -2555,7 +2568,7 @@
     <row r="32">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
-      <c r="D32" s="14"/>
+      <c r="D32" s="13"/>
       <c r="E32" s="5"/>
       <c r="J32" s="6"/>
       <c r="K32" s="2"/>
@@ -2580,7 +2593,7 @@
       <c r="AA33" s="2"/>
       <c r="AB33" s="2"/>
       <c r="AC33" s="2"/>
-      <c r="AD33" s="14"/>
+      <c r="AD33" s="13"/>
       <c r="AE33" s="5"/>
       <c r="AF33" s="2"/>
       <c r="AG33" s="2"/>
@@ -2595,14 +2608,14 @@
     <row r="34">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
-      <c r="D34" s="14"/>
+      <c r="D34" s="13"/>
       <c r="E34" s="5"/>
       <c r="J34" s="6"/>
       <c r="K34" s="2"/>
       <c r="AA34" s="2"/>
       <c r="AB34" s="2"/>
       <c r="AC34" s="2"/>
-      <c r="AD34" s="14"/>
+      <c r="AD34" s="13"/>
       <c r="AE34" s="5"/>
       <c r="AF34" s="2"/>
       <c r="AG34" s="2"/>
@@ -2620,12 +2633,12 @@
       <c r="D35" s="2"/>
       <c r="E35" s="5"/>
       <c r="H35" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="I35" s="1"/>
       <c r="J35" s="6">
         <f>SUM(J3:J32)</f>
-        <v>97.410000000000011</v>
+        <v>97.579999999999998</v>
       </c>
       <c r="K35" s="23"/>
       <c r="AA35" s="2"/>
@@ -2646,20 +2659,20 @@
     <row r="36">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
-      <c r="D36" s="18"/>
+      <c r="D36" s="17"/>
       <c r="E36" s="5"/>
       <c r="H36" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I36" s="1"/>
       <c r="J36">
         <f>SUM(K3:K32)</f>
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="AA36" s="2"/>
       <c r="AB36" s="2"/>
       <c r="AC36" s="2"/>
-      <c r="AD36" s="18"/>
+      <c r="AD36" s="17"/>
       <c r="AE36" s="5"/>
       <c r="AF36" s="2"/>
       <c r="AG36" s="2"/>
@@ -2697,12 +2710,12 @@
       <c r="D38" s="2"/>
       <c r="E38" s="5"/>
       <c r="H38" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I38" s="1"/>
       <c r="J38" s="6">
         <f>J35/C1</f>
-        <v>97.410000000000011</v>
+        <v>97.579999999999998</v>
       </c>
       <c r="AA38" s="2"/>
       <c r="AB38" s="2"/>
@@ -2725,12 +2738,12 @@
       <c r="D39" s="2"/>
       <c r="E39" s="5"/>
       <c r="H39" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="I39" s="1"/>
       <c r="J39">
         <f>J36/C1</f>
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="AA39" s="2"/>
       <c r="AB39" s="2"/>
@@ -2773,7 +2786,14 @@
       <c r="B41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="5"/>
-      <c r="J41" s="6"/>
+      <c r="H41" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="I41" s="24"/>
+      <c r="J41" s="25">
+        <f>SUM(B3:B28)</f>
+        <v>70</v>
+      </c>
       <c r="AA41" s="2"/>
       <c r="AB41" s="2"/>
       <c r="AC41" s="2"/>
@@ -2794,7 +2814,14 @@
       <c r="B42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="5"/>
-      <c r="J42" s="6"/>
+      <c r="H42" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="I42" s="1"/>
+      <c r="J42" s="27">
+        <f>J41/J39</f>
+        <v>0.69999999999999996</v>
+      </c>
       <c r="AA42" s="2"/>
       <c r="AB42" s="2"/>
       <c r="AC42" s="2"/>
@@ -2918,12 +2945,12 @@
     <row r="48">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
-      <c r="D48" s="24"/>
+      <c r="D48" s="28"/>
       <c r="J48" s="6"/>
       <c r="AA48" s="2"/>
       <c r="AB48" s="2"/>
       <c r="AC48" s="2"/>
-      <c r="AD48" s="24"/>
+      <c r="AD48" s="28"/>
       <c r="AE48" s="2"/>
       <c r="AF48" s="2"/>
       <c r="AG48" s="2"/>
@@ -3052,11 +3079,11 @@
     <row r="55">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
-      <c r="D55" s="24"/>
+      <c r="D55" s="28"/>
       <c r="AA55" s="2"/>
       <c r="AB55" s="2"/>
       <c r="AC55" s="2"/>
-      <c r="AD55" s="24"/>
+      <c r="AD55" s="28"/>
       <c r="AE55" s="2"/>
       <c r="AF55" s="2"/>
       <c r="AG55" s="2"/>
@@ -3216,13 +3243,15 @@
       <c r="AN64" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="AA1:AB1"/>
     <mergeCell ref="H35:I35"/>
     <mergeCell ref="H36:I36"/>
     <mergeCell ref="H38:I38"/>
     <mergeCell ref="H39:I39"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="H42:I42"/>
     <mergeCell ref="AH53:AI53"/>
     <mergeCell ref="AH54:AI54"/>
     <mergeCell ref="AH56:AI56"/>
@@ -3243,19 +3272,17 @@
     <hyperlink r:id="rId12" ref="E14"/>
     <hyperlink r:id="rId13" ref="E15"/>
     <hyperlink r:id="rId14" ref="E16"/>
-    <hyperlink r:id="rId13" ref="E17"/>
-    <hyperlink r:id="rId15" ref="E18"/>
-    <hyperlink r:id="rId16" ref="E19"/>
-    <hyperlink r:id="rId17" ref="E20"/>
-    <hyperlink r:id="rId18" ref="E21"/>
-    <hyperlink r:id="rId19" ref="E22"/>
-    <hyperlink r:id="rId20" ref="E23"/>
-    <hyperlink r:id="rId21" ref="E24"/>
-    <hyperlink r:id="rId22" ref="E25"/>
-    <hyperlink r:id="rId23" ref="E26"/>
-    <hyperlink r:id="rId24" ref="E27"/>
-    <hyperlink r:id="rId25" ref="E28"/>
-    <hyperlink r:id="rId26" ref="E29"/>
+    <hyperlink r:id="rId15" ref="E17"/>
+    <hyperlink r:id="rId16" ref="E18"/>
+    <hyperlink r:id="rId17" ref="E19"/>
+    <hyperlink r:id="rId18" ref="E20"/>
+    <hyperlink r:id="rId19" ref="E21"/>
+    <hyperlink r:id="rId20" ref="E22"/>
+    <hyperlink r:id="rId21" ref="E23"/>
+    <hyperlink r:id="rId22" ref="E24"/>
+    <hyperlink r:id="rId23" ref="E25"/>
+    <hyperlink r:id="rId24" ref="E26"/>
+    <hyperlink r:id="rId25" ref="E27"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
Did design review, just need to debug pyro channel
Changed pull resistor on the pyro channel from 1k to 10k during design review
</commit_message>
<xml_diff>
--- a/PCB/Output/BOM.xlsx
+++ b/PCB/Output/BOM.xlsx
@@ -1054,11 +1054,11 @@
         <v>0.0064000000000000003</v>
       </c>
       <c r="J3" s="6">
-        <f t="shared" ref="J3:J9" si="1">IF(MIN(IF(I3=0,1000000,I3*ROUNDUP(C3,-3)),IF(H3=0,1000000,H3*ROUNDUP(C3,-2)),IF(G3=0,1000000,G3*ROUNDUP(C3,-1)),IF(F3=0,1000000,F3*C3))=1000000,0,MIN(IF(I3=0,1000000,I3*ROUNDUP(C3,-3)),IF(H3=0,1000000,H3*ROUNDUP(C3,-2)),IF(G3=0,1000000,G3*ROUNDUP(C3,-1)),IF(F3=0,1000000,F3*C3)))</f>
+        <f>IF(MIN(IF(I3=0,1000000,I3*ROUNDUP(C3,-3)),IF(H3=0,1000000,H3*ROUNDUP(C3,-2)),IF(G3=0,1000000,G3*ROUNDUP(C3,-1)),IF(F3=0,1000000,F3*C3))=1000000,0,MIN(IF(I3=0,1000000,I3*ROUNDUP(C3,-3)),IF(H3=0,1000000,H3*ROUNDUP(C3,-2)),IF(G3=0,1000000,G3*ROUNDUP(C3,-1)),IF(F3=0,1000000,F3*C3)))</f>
         <v>0.28000000000000003</v>
       </c>
       <c r="K3" s="2">
-        <f t="shared" ref="K3:K9" si="2">IF(J3=IF(F3=0,1000000,F3*C3),C3,IF(J3=IF(G3=0,1000000,G3*ROUNDUP(C3,-1)),ROUNDUP(C3,-1),IF(J3=IF(H3=0,1000000,H3*ROUNDUP(C3,-2)),ROUNDUP(C3,-2),IF(J3=IF(I3=0,1000000,I3*ROUNDUP(C3,-3)),ROUNDUP(C3,-3),0))))</f>
+        <f t="shared" ref="K3:K9" si="1">IF(J3=IF(F3=0,1000000,F3*C3),C3,IF(J3=IF(G3=0,1000000,G3*ROUNDUP(C3,-1)),ROUNDUP(C3,-1),IF(J3=IF(H3=0,1000000,H3*ROUNDUP(C3,-2)),ROUNDUP(C3,-2),IF(J3=IF(I3=0,1000000,I3*ROUNDUP(C3,-3)),ROUNDUP(C3,-3),0))))</f>
         <v>20</v>
       </c>
       <c r="L3" s="2" t="s">
@@ -1117,11 +1117,11 @@
         <v>0.0064000000000000003</v>
       </c>
       <c r="J4" s="6">
+        <f t="shared" ref="J4:J9" si="2">IF(MIN(IF(I4=0,1000000,I4*ROUNDUP(C4,-3)),IF(H4=0,1000000,H4*ROUNDUP(C4,-2)),IF(G4=0,1000000,G4*ROUNDUP(C4,-1)),IF(F4=0,1000000,F4*C4))=1000000,0,MIN(IF(I4=0,1000000,I4*ROUNDUP(C4,-3)),IF(H4=0,1000000,H4*ROUNDUP(C4,-2)),IF(G4=0,1000000,G4*ROUNDUP(C4,-1)),IF(F4=0,1000000,F4*C4)))</f>
+        <v>0.01</v>
+      </c>
+      <c r="K4" s="2">
         <f t="shared" si="1"/>
-        <v>0.01</v>
-      </c>
-      <c r="K4" s="2">
-        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="L4" s="2" t="s">
@@ -1171,11 +1171,11 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="6">
+        <f t="shared" si="2"/>
+        <v>0.050000000000000003</v>
+      </c>
+      <c r="K5" s="2">
         <f t="shared" si="1"/>
-        <v>0.050000000000000003</v>
-      </c>
-      <c r="K5" s="2">
-        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="L5" s="2" t="s">
@@ -1225,11 +1225,11 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="6">
+        <f t="shared" si="2"/>
+        <v>0.20000000000000001</v>
+      </c>
+      <c r="K6" s="2">
         <f t="shared" si="1"/>
-        <v>0.20000000000000001</v>
-      </c>
-      <c r="K6" s="2">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="L6" s="2" t="s">
@@ -1277,11 +1277,11 @@
         <v>0.84999999999999998</v>
       </c>
       <c r="J7" s="6">
+        <f t="shared" si="2"/>
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="K7" s="2">
         <f t="shared" si="1"/>
-        <v>0.10000000000000001</v>
-      </c>
-      <c r="K7" s="2">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L7" t="s">
@@ -1333,11 +1333,11 @@
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="6">
+        <f t="shared" si="2"/>
+        <v>0.78000000000000003</v>
+      </c>
+      <c r="K8" s="2">
         <f t="shared" si="1"/>
-        <v>0.78000000000000003</v>
-      </c>
-      <c r="K8" s="2">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L8" s="2" t="s">
@@ -1391,11 +1391,11 @@
         <v>0.96562999999999999</v>
       </c>
       <c r="J9" s="6">
+        <f t="shared" si="2"/>
+        <v>2.3500000000000001</v>
+      </c>
+      <c r="K9" s="2">
         <f t="shared" si="1"/>
-        <v>2.3500000000000001</v>
-      </c>
-      <c r="K9" s="2">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L9" t="s">
@@ -1598,11 +1598,11 @@
         <v>52</v>
       </c>
       <c r="B13" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C13" s="2">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D13" s="12">
         <v>1</v>
@@ -1656,11 +1656,11 @@
         <v>55</v>
       </c>
       <c r="B14" s="2">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C14" s="2">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D14" s="14">
         <v>10</v>

</xml_diff>

<commit_message>
Cleaned up schematic Change from SPI and I2C to busses
</commit_message>
<xml_diff>
--- a/PCB/Output/BOM.xlsx
+++ b/PCB/Output/BOM.xlsx
@@ -318,13 +318,13 @@
     <t>U701,U702,U703</t>
   </si>
   <si>
-    <t>~</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/rohm-semiconductor/UT6MA3TCR/6573278?s=N4IgTCBcDaIKoBUBsBZAggZgQYQEogF0BfIA</t>
-  </si>
-  <si>
-    <t>UT6MA3TCRCT-ND</t>
+    <t>UT6ME5TCR</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/rohm-semiconductor/UT6ME5TCR/20516416</t>
+  </si>
+  <si>
+    <t>846-UT6ME5TCRCT-ND</t>
   </si>
   <si>
     <t>Y301</t>
@@ -1054,11 +1054,11 @@
         <v>0.0064000000000000003</v>
       </c>
       <c r="J3" s="6">
-        <f>IF(MIN(IF(I3=0,1000000,I3*ROUNDUP(C3,-3)),IF(H3=0,1000000,H3*ROUNDUP(C3,-2)),IF(G3=0,1000000,G3*ROUNDUP(C3,-1)),IF(F3=0,1000000,F3*C3))=1000000,0,MIN(IF(I3=0,1000000,I3*ROUNDUP(C3,-3)),IF(H3=0,1000000,H3*ROUNDUP(C3,-2)),IF(G3=0,1000000,G3*ROUNDUP(C3,-1)),IF(F3=0,1000000,F3*C3)))</f>
+        <f t="shared" ref="J3:J9" si="1">IF(MIN(IF(I3=0,1000000,I3*ROUNDUP(C3,-3)),IF(H3=0,1000000,H3*ROUNDUP(C3,-2)),IF(G3=0,1000000,G3*ROUNDUP(C3,-1)),IF(F3=0,1000000,F3*C3))=1000000,0,MIN(IF(I3=0,1000000,I3*ROUNDUP(C3,-3)),IF(H3=0,1000000,H3*ROUNDUP(C3,-2)),IF(G3=0,1000000,G3*ROUNDUP(C3,-1)),IF(F3=0,1000000,F3*C3)))</f>
         <v>0.28000000000000003</v>
       </c>
       <c r="K3" s="2">
-        <f t="shared" ref="K3:K9" si="1">IF(J3=IF(F3=0,1000000,F3*C3),C3,IF(J3=IF(G3=0,1000000,G3*ROUNDUP(C3,-1)),ROUNDUP(C3,-1),IF(J3=IF(H3=0,1000000,H3*ROUNDUP(C3,-2)),ROUNDUP(C3,-2),IF(J3=IF(I3=0,1000000,I3*ROUNDUP(C3,-3)),ROUNDUP(C3,-3),0))))</f>
+        <f t="shared" ref="K3:K9" si="2">IF(J3=IF(F3=0,1000000,F3*C3),C3,IF(J3=IF(G3=0,1000000,G3*ROUNDUP(C3,-1)),ROUNDUP(C3,-1),IF(J3=IF(H3=0,1000000,H3*ROUNDUP(C3,-2)),ROUNDUP(C3,-2),IF(J3=IF(I3=0,1000000,I3*ROUNDUP(C3,-3)),ROUNDUP(C3,-3),0))))</f>
         <v>20</v>
       </c>
       <c r="L3" s="2" t="s">
@@ -1117,11 +1117,11 @@
         <v>0.0064000000000000003</v>
       </c>
       <c r="J4" s="6">
-        <f t="shared" ref="J4:J9" si="2">IF(MIN(IF(I4=0,1000000,I4*ROUNDUP(C4,-3)),IF(H4=0,1000000,H4*ROUNDUP(C4,-2)),IF(G4=0,1000000,G4*ROUNDUP(C4,-1)),IF(F4=0,1000000,F4*C4))=1000000,0,MIN(IF(I4=0,1000000,I4*ROUNDUP(C4,-3)),IF(H4=0,1000000,H4*ROUNDUP(C4,-2)),IF(G4=0,1000000,G4*ROUNDUP(C4,-1)),IF(F4=0,1000000,F4*C4)))</f>
+        <f t="shared" si="1"/>
         <v>0.01</v>
       </c>
       <c r="K4" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="L4" s="2" t="s">
@@ -1171,11 +1171,11 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="6">
+        <f t="shared" si="1"/>
+        <v>0.050000000000000003</v>
+      </c>
+      <c r="K5" s="2">
         <f t="shared" si="2"/>
-        <v>0.050000000000000003</v>
-      </c>
-      <c r="K5" s="2">
-        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="L5" s="2" t="s">
@@ -1225,11 +1225,11 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="6">
+        <f t="shared" si="1"/>
+        <v>0.20000000000000001</v>
+      </c>
+      <c r="K6" s="2">
         <f t="shared" si="2"/>
-        <v>0.20000000000000001</v>
-      </c>
-      <c r="K6" s="2">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="L6" s="2" t="s">
@@ -1277,11 +1277,11 @@
         <v>0.84999999999999998</v>
       </c>
       <c r="J7" s="6">
+        <f t="shared" si="1"/>
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="K7" s="2">
         <f t="shared" si="2"/>
-        <v>0.10000000000000001</v>
-      </c>
-      <c r="K7" s="2">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L7" t="s">
@@ -1333,11 +1333,11 @@
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="6">
+        <f t="shared" si="1"/>
+        <v>0.78000000000000003</v>
+      </c>
+      <c r="K8" s="2">
         <f t="shared" si="2"/>
-        <v>0.78000000000000003</v>
-      </c>
-      <c r="K8" s="2">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L8" s="2" t="s">
@@ -1391,11 +1391,11 @@
         <v>0.96562999999999999</v>
       </c>
       <c r="J9" s="6">
+        <f t="shared" si="1"/>
+        <v>2.3500000000000001</v>
+      </c>
+      <c r="K9" s="2">
         <f t="shared" si="2"/>
-        <v>2.3500000000000001</v>
-      </c>
-      <c r="K9" s="2">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L9" t="s">
@@ -2350,20 +2350,20 @@
         <v>101</v>
       </c>
       <c r="F26" s="2">
-        <v>1.3200000000000001</v>
+        <v>0.46999999999999997</v>
       </c>
       <c r="G26" s="2">
-        <v>0.85099999999999998</v>
+        <v>0.32900000000000001</v>
       </c>
       <c r="H26" s="2">
-        <v>0.56289999999999996</v>
+        <v>0.25490000000000002</v>
       </c>
       <c r="I26" s="2">
-        <v>0.39964</v>
+        <v>0.21598999999999999</v>
       </c>
       <c r="J26" s="6">
         <f t="shared" si="4"/>
-        <v>3.96</v>
+        <v>1.4099999999999999</v>
       </c>
       <c r="K26" s="2">
         <f t="shared" si="5"/>
@@ -2625,7 +2625,7 @@
       <c r="I35" s="1"/>
       <c r="J35" s="6">
         <f>SUM(J3:J32)</f>
-        <v>96.820000000000007</v>
+        <v>94.27000000000001</v>
       </c>
       <c r="K35" s="22"/>
       <c r="AA35" s="2"/>
@@ -2702,7 +2702,7 @@
       <c r="I38" s="1"/>
       <c r="J38" s="6">
         <f>J35/C1</f>
-        <v>96.820000000000007</v>
+        <v>94.27000000000001</v>
       </c>
       <c r="AA38" s="2"/>
       <c r="AB38" s="2"/>

</xml_diff>

<commit_message>
Fixed component annotation Updated BOM to reflect the pyro channel changes Updates Production files
</commit_message>
<xml_diff>
--- a/PCB/Output/BOM.xlsx
+++ b/PCB/Output/BOM.xlsx
@@ -174,7 +174,19 @@
     <t>CON-SMA-EDGE-S-ND</t>
   </si>
   <si>
-    <t>R201,R202,R701,R705,R708,R713</t>
+    <t>Q701,Q702,Q703</t>
+  </si>
+  <si>
+    <t>SL2302S</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/shenzhen-slkormicro-semicon-co-ltd/SL2302S/26112886?s=N4IgTCBcDaIMoBkwGYAMY4gLoF8g</t>
+  </si>
+  <si>
+    <t>5399-SL2302STR-ND</t>
+  </si>
+  <si>
+    <t>R201,R202,R704</t>
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0603FT1K00/1761077</t>
@@ -183,7 +195,7 @@
     <t>RMCF0603FT1K00CT-ND</t>
   </si>
   <si>
-    <t>R301,R302,R401,R402,R702,R703,R707,R709,R712,R714,R717</t>
+    <t>R301,R302,R401,R402,R701,R705,R709,R713</t>
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0603JT10K0/1758104</t>
@@ -192,7 +204,7 @@
     <t>RMCF0603JT10K0CT-ND</t>
   </si>
   <si>
-    <t>R303,R304,R501,R502,R718,R720,R722</t>
+    <t>R303,R304,R501,R502,R703,R708,R712</t>
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/yageo/RC0603FR-075K1L/727268</t>
@@ -201,7 +213,7 @@
     <t>311-5.10KHRCT-ND</t>
   </si>
   <si>
-    <t>R704,R710,R715</t>
+    <t>R702,R707,R711</t>
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/yageo/RT0603BRD07500RL/17019950</t>
@@ -210,7 +222,7 @@
     <t>13-RT0603BRD07500RLCT-ND</t>
   </si>
   <si>
-    <t>R706,R711,R716,R719,R721,R723</t>
+    <t>R706,R710,R714</t>
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/panasonic-electronic-components/ERA-3AEB302V/1465865</t>
@@ -313,18 +325,6 @@
   </si>
   <si>
     <t>1597-1488-ND</t>
-  </si>
-  <si>
-    <t>U701,U702,U703</t>
-  </si>
-  <si>
-    <t>UT6ME5TCR</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/rohm-semiconductor/UT6ME5TCR/20516416</t>
-  </si>
-  <si>
-    <t>846-UT6ME5TCRCT-ND</t>
   </si>
   <si>
     <t>Y301</t>
@@ -425,7 +425,7 @@
     <xf fontId="0" fillId="2" borderId="0" numFmtId="44" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -434,20 +434,39 @@
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="165" xfId="1" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="166" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="166" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="167" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="168" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="169" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="170" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="171" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="172" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="171" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="173" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="174" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="173" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="175" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="176" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="175" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="177" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="178" xfId="0" applyNumberFormat="1"/>
@@ -1054,11 +1073,11 @@
         <v>0.0064000000000000003</v>
       </c>
       <c r="J3" s="6">
-        <f t="shared" ref="J3:J9" si="1">IF(MIN(IF(I3=0,1000000,I3*ROUNDUP(C3,-3)),IF(H3=0,1000000,H3*ROUNDUP(C3,-2)),IF(G3=0,1000000,G3*ROUNDUP(C3,-1)),IF(F3=0,1000000,F3*C3))=1000000,0,MIN(IF(I3=0,1000000,I3*ROUNDUP(C3,-3)),IF(H3=0,1000000,H3*ROUNDUP(C3,-2)),IF(G3=0,1000000,G3*ROUNDUP(C3,-1)),IF(F3=0,1000000,F3*C3)))</f>
+        <f>IF(MIN(IF(I3=0,1000000,I3*ROUNDUP(C3,-3)),IF(H3=0,1000000,H3*ROUNDUP(C3,-2)),IF(G3=0,1000000,G3*ROUNDUP(C3,-1)),IF(F3=0,1000000,F3*C3))=1000000,0,MIN(IF(I3=0,1000000,I3*ROUNDUP(C3,-3)),IF(H3=0,1000000,H3*ROUNDUP(C3,-2)),IF(G3=0,1000000,G3*ROUNDUP(C3,-1)),IF(F3=0,1000000,F3*C3)))</f>
         <v>0.28000000000000003</v>
       </c>
       <c r="K3" s="2">
-        <f t="shared" ref="K3:K9" si="2">IF(J3=IF(F3=0,1000000,F3*C3),C3,IF(J3=IF(G3=0,1000000,G3*ROUNDUP(C3,-1)),ROUNDUP(C3,-1),IF(J3=IF(H3=0,1000000,H3*ROUNDUP(C3,-2)),ROUNDUP(C3,-2),IF(J3=IF(I3=0,1000000,I3*ROUNDUP(C3,-3)),ROUNDUP(C3,-3),0))))</f>
+        <f>IF(J3=IF(F3=0,1000000,F3*C3),C3,IF(J3=IF(G3=0,1000000,G3*ROUNDUP(C3,-1)),ROUNDUP(C3,-1),IF(J3=IF(H3=0,1000000,H3*ROUNDUP(C3,-2)),ROUNDUP(C3,-2),IF(J3=IF(I3=0,1000000,I3*ROUNDUP(C3,-3)),ROUNDUP(C3,-3),0))))</f>
         <v>20</v>
       </c>
       <c r="L3" s="2" t="s">
@@ -1071,11 +1090,11 @@
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
-      <c r="R3" s="4"/>
+      <c r="R3" s="7"/>
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
       <c r="AC3" s="2"/>
-      <c r="AD3" s="4"/>
+      <c r="AD3" s="7"/>
       <c r="AE3" s="5"/>
       <c r="AF3" s="2"/>
       <c r="AG3" s="2"/>
@@ -1117,11 +1136,11 @@
         <v>0.0064000000000000003</v>
       </c>
       <c r="J4" s="6">
-        <f t="shared" si="1"/>
+        <f>IF(MIN(IF(I4=0,1000000,I4*ROUNDUP(C4,-3)),IF(H4=0,1000000,H4*ROUNDUP(C4,-2)),IF(G4=0,1000000,G4*ROUNDUP(C4,-1)),IF(F4=0,1000000,F4*C4))=1000000,0,MIN(IF(I4=0,1000000,I4*ROUNDUP(C4,-3)),IF(H4=0,1000000,H4*ROUNDUP(C4,-2)),IF(G4=0,1000000,G4*ROUNDUP(C4,-1)),IF(F4=0,1000000,F4*C4)))</f>
         <v>0.01</v>
       </c>
       <c r="K4" s="2">
-        <f t="shared" si="2"/>
+        <f>IF(J4=IF(F4=0,1000000,F4*C4),C4,IF(J4=IF(G4=0,1000000,G4*ROUNDUP(C4,-1)),ROUNDUP(C4,-1),IF(J4=IF(H4=0,1000000,H4*ROUNDUP(C4,-2)),ROUNDUP(C4,-2),IF(J4=IF(I4=0,1000000,I4*ROUNDUP(C4,-3)),ROUNDUP(C4,-3),0))))</f>
         <v>10</v>
       </c>
       <c r="L4" s="2" t="s">
@@ -1129,11 +1148,11 @@
       </c>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
-      <c r="R4" s="4"/>
+      <c r="R4" s="7"/>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
       <c r="AC4" s="2"/>
-      <c r="AD4" s="7"/>
+      <c r="AD4" s="8"/>
       <c r="AE4" s="5"/>
       <c r="AF4" s="2"/>
       <c r="AG4" s="2"/>
@@ -1156,7 +1175,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="9">
         <v>1</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -1171,11 +1190,11 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="6">
-        <f t="shared" si="1"/>
+        <f>IF(MIN(IF(I5=0,1000000,I5*ROUNDUP(C5,-3)),IF(H5=0,1000000,H5*ROUNDUP(C5,-2)),IF(G5=0,1000000,G5*ROUNDUP(C5,-1)),IF(F5=0,1000000,F5*C5))=1000000,0,MIN(IF(I5=0,1000000,I5*ROUNDUP(C5,-3)),IF(H5=0,1000000,H5*ROUNDUP(C5,-2)),IF(G5=0,1000000,G5*ROUNDUP(C5,-1)),IF(F5=0,1000000,F5*C5)))</f>
         <v>0.050000000000000003</v>
       </c>
       <c r="K5" s="2">
-        <f t="shared" si="2"/>
+        <f>IF(J5=IF(F5=0,1000000,F5*C5),C5,IF(J5=IF(G5=0,1000000,G5*ROUNDUP(C5,-1)),ROUNDUP(C5,-1),IF(J5=IF(H5=0,1000000,H5*ROUNDUP(C5,-2)),ROUNDUP(C5,-2),IF(J5=IF(I5=0,1000000,I5*ROUNDUP(C5,-3)),ROUNDUP(C5,-3),0))))</f>
         <v>10</v>
       </c>
       <c r="L5" s="2" t="s">
@@ -1183,11 +1202,11 @@
       </c>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
-      <c r="R5" s="7"/>
+      <c r="R5" s="8"/>
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
-      <c r="AD5" s="4"/>
+      <c r="AD5" s="7"/>
       <c r="AE5" s="5"/>
       <c r="AF5" s="2"/>
       <c r="AG5" s="2"/>
@@ -1210,7 +1229,7 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="10" t="s">
         <v>25</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -1225,11 +1244,11 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="6">
-        <f t="shared" si="1"/>
+        <f>IF(MIN(IF(I6=0,1000000,I6*ROUNDUP(C6,-3)),IF(H6=0,1000000,H6*ROUNDUP(C6,-2)),IF(G6=0,1000000,G6*ROUNDUP(C6,-1)),IF(F6=0,1000000,F6*C6))=1000000,0,MIN(IF(I6=0,1000000,I6*ROUNDUP(C6,-3)),IF(H6=0,1000000,H6*ROUNDUP(C6,-2)),IF(G6=0,1000000,G6*ROUNDUP(C6,-1)),IF(F6=0,1000000,F6*C6)))</f>
         <v>0.20000000000000001</v>
       </c>
       <c r="K6" s="2">
-        <f t="shared" si="2"/>
+        <f>IF(J6=IF(F6=0,1000000,F6*C6),C6,IF(J6=IF(G6=0,1000000,G6*ROUNDUP(C6,-1)),ROUNDUP(C6,-1),IF(J6=IF(H6=0,1000000,H6*ROUNDUP(C6,-2)),ROUNDUP(C6,-2),IF(J6=IF(I6=0,1000000,I6*ROUNDUP(C6,-3)),ROUNDUP(C6,-3),0))))</f>
         <v>2</v>
       </c>
       <c r="L6" s="2" t="s">
@@ -1241,7 +1260,7 @@
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
-      <c r="AD6" s="8"/>
+      <c r="AD6" s="11"/>
       <c r="AE6" s="5"/>
       <c r="AF6" s="2"/>
       <c r="AG6" s="2"/>
@@ -1264,7 +1283,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="10" t="s">
         <v>29</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -1277,11 +1296,11 @@
         <v>0.84999999999999998</v>
       </c>
       <c r="J7" s="6">
-        <f t="shared" si="1"/>
+        <f>IF(MIN(IF(I7=0,1000000,I7*ROUNDUP(C7,-3)),IF(H7=0,1000000,H7*ROUNDUP(C7,-2)),IF(G7=0,1000000,G7*ROUNDUP(C7,-1)),IF(F7=0,1000000,F7*C7))=1000000,0,MIN(IF(I7=0,1000000,I7*ROUNDUP(C7,-3)),IF(H7=0,1000000,H7*ROUNDUP(C7,-2)),IF(G7=0,1000000,G7*ROUNDUP(C7,-1)),IF(F7=0,1000000,F7*C7)))</f>
         <v>0.10000000000000001</v>
       </c>
       <c r="K7" s="2">
-        <f t="shared" si="2"/>
+        <f>IF(J7=IF(F7=0,1000000,F7*C7),C7,IF(J7=IF(G7=0,1000000,G7*ROUNDUP(C7,-1)),ROUNDUP(C7,-1),IF(J7=IF(H7=0,1000000,H7*ROUNDUP(C7,-2)),ROUNDUP(C7,-2),IF(J7=IF(I7=0,1000000,I7*ROUNDUP(C7,-3)),ROUNDUP(C7,-3),0))))</f>
         <v>1</v>
       </c>
       <c r="L7" t="s">
@@ -1293,7 +1312,7 @@
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
-      <c r="AD7" s="9"/>
+      <c r="AD7" s="12"/>
       <c r="AE7" s="5"/>
       <c r="AF7" s="2"/>
       <c r="AG7" s="2"/>
@@ -1316,7 +1335,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="10" t="s">
         <v>33</v>
       </c>
       <c r="E8" s="5" t="s">
@@ -1333,11 +1352,11 @@
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="6">
-        <f t="shared" si="1"/>
+        <f>IF(MIN(IF(I8=0,1000000,I8*ROUNDUP(C8,-3)),IF(H8=0,1000000,H8*ROUNDUP(C8,-2)),IF(G8=0,1000000,G8*ROUNDUP(C8,-1)),IF(F8=0,1000000,F8*C8))=1000000,0,MIN(IF(I8=0,1000000,I8*ROUNDUP(C8,-3)),IF(H8=0,1000000,H8*ROUNDUP(C8,-2)),IF(G8=0,1000000,G8*ROUNDUP(C8,-1)),IF(F8=0,1000000,F8*C8)))</f>
         <v>0.78000000000000003</v>
       </c>
       <c r="K8" s="2">
-        <f t="shared" si="2"/>
+        <f>IF(J8=IF(F8=0,1000000,F8*C8),C8,IF(J8=IF(G8=0,1000000,G8*ROUNDUP(C8,-1)),ROUNDUP(C8,-1),IF(J8=IF(H8=0,1000000,H8*ROUNDUP(C8,-2)),ROUNDUP(C8,-2),IF(J8=IF(I8=0,1000000,I8*ROUNDUP(C8,-3)),ROUNDUP(C8,-3),0))))</f>
         <v>1</v>
       </c>
       <c r="L8" s="2" t="s">
@@ -1349,7 +1368,7 @@
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
-      <c r="AD8" s="10"/>
+      <c r="AD8" s="13"/>
       <c r="AE8" s="5"/>
       <c r="AF8" s="2"/>
       <c r="AG8" s="2"/>
@@ -1372,7 +1391,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="10" t="s">
         <v>37</v>
       </c>
       <c r="E9" s="5" t="s">
@@ -1391,11 +1410,11 @@
         <v>0.96562999999999999</v>
       </c>
       <c r="J9" s="6">
-        <f t="shared" si="1"/>
+        <f>IF(MIN(IF(I9=0,1000000,I9*ROUNDUP(C9,-3)),IF(H9=0,1000000,H9*ROUNDUP(C9,-2)),IF(G9=0,1000000,G9*ROUNDUP(C9,-1)),IF(F9=0,1000000,F9*C9))=1000000,0,MIN(IF(I9=0,1000000,I9*ROUNDUP(C9,-3)),IF(H9=0,1000000,H9*ROUNDUP(C9,-2)),IF(G9=0,1000000,G9*ROUNDUP(C9,-1)),IF(F9=0,1000000,F9*C9)))</f>
         <v>2.3500000000000001</v>
       </c>
       <c r="K9" s="2">
-        <f t="shared" si="2"/>
+        <f>IF(J9=IF(F9=0,1000000,F9*C9),C9,IF(J9=IF(G9=0,1000000,G9*ROUNDUP(C9,-1)),ROUNDUP(C9,-1),IF(J9=IF(H9=0,1000000,H9*ROUNDUP(C9,-2)),ROUNDUP(C9,-2),IF(J9=IF(I9=0,1000000,I9*ROUNDUP(C9,-3)),ROUNDUP(C9,-3),0))))</f>
         <v>1</v>
       </c>
       <c r="L9" t="s">
@@ -1407,7 +1426,7 @@
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
-      <c r="AD9" s="11"/>
+      <c r="AD9" s="14"/>
       <c r="AE9" s="5"/>
       <c r="AF9" s="2"/>
       <c r="AG9" s="2"/>
@@ -1427,10 +1446,10 @@
         <v>1</v>
       </c>
       <c r="C10" s="2">
-        <f t="shared" ref="C10:C28" si="3">$C$1*B10</f>
-        <v>1</v>
-      </c>
-      <c r="D10" s="2" t="s">
+        <f t="shared" ref="C10:C28" si="1">$C$1*B10</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>41</v>
       </c>
       <c r="E10" s="5" t="s">
@@ -1449,11 +1468,11 @@
         <v>0.65947999999999996</v>
       </c>
       <c r="J10" s="6">
-        <f t="shared" ref="J10:J28" si="4">IF(MIN(IF(I10=0,1000000,I10*ROUNDUP(C10,-3)),IF(H10=0,1000000,H10*ROUNDUP(C10,-2)),IF(G10=0,1000000,G10*ROUNDUP(C10,-1)),IF(F10=0,1000000,F10*C10))=1000000,0,MIN(IF(I10=0,1000000,I10*ROUNDUP(C10,-3)),IF(H10=0,1000000,H10*ROUNDUP(C10,-2)),IF(G10=0,1000000,G10*ROUNDUP(C10,-1)),IF(F10=0,1000000,F10*C10)))</f>
+        <f>IF(MIN(IF(I10=0,1000000,I10*ROUNDUP(C10,-3)),IF(H10=0,1000000,H10*ROUNDUP(C10,-2)),IF(G10=0,1000000,G10*ROUNDUP(C10,-1)),IF(F10=0,1000000,F10*C10))=1000000,0,MIN(IF(I10=0,1000000,I10*ROUNDUP(C10,-3)),IF(H10=0,1000000,H10*ROUNDUP(C10,-2)),IF(G10=0,1000000,G10*ROUNDUP(C10,-1)),IF(F10=0,1000000,F10*C10)))</f>
         <v>1.6299999999999999</v>
       </c>
       <c r="K10" s="2">
-        <f t="shared" ref="K10:K28" si="5">IF(J10=IF(F10=0,1000000,F10*C10),C10,IF(J10=IF(G10=0,1000000,G10*ROUNDUP(C10,-1)),ROUNDUP(C10,-1),IF(J10=IF(H10=0,1000000,H10*ROUNDUP(C10,-2)),ROUNDUP(C10,-2),IF(J10=IF(I10=0,1000000,I10*ROUNDUP(C10,-3)),ROUNDUP(C10,-3),0))))</f>
+        <f>IF(J10=IF(F10=0,1000000,F10*C10),C10,IF(J10=IF(G10=0,1000000,G10*ROUNDUP(C10,-1)),ROUNDUP(C10,-1),IF(J10=IF(H10=0,1000000,H10*ROUNDUP(C10,-2)),ROUNDUP(C10,-2),IF(J10=IF(I10=0,1000000,I10*ROUNDUP(C10,-3)),ROUNDUP(C10,-3),0))))</f>
         <v>1</v>
       </c>
       <c r="L10" t="s">
@@ -1465,7 +1484,7 @@
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
-      <c r="AD10" s="8"/>
+      <c r="AD10" s="11"/>
       <c r="AE10" s="5"/>
       <c r="AF10" s="2"/>
       <c r="AG10" s="2"/>
@@ -1485,10 +1504,10 @@
         <v>1</v>
       </c>
       <c r="C11" s="2">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D11" s="2" t="s">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>45</v>
       </c>
       <c r="E11" s="5" t="s">
@@ -1507,11 +1526,11 @@
         <v>0.30617</v>
       </c>
       <c r="J11" s="6">
-        <f t="shared" si="4"/>
+        <f>IF(MIN(IF(I11=0,1000000,I11*ROUNDUP(C11,-3)),IF(H11=0,1000000,H11*ROUNDUP(C11,-2)),IF(G11=0,1000000,G11*ROUNDUP(C11,-1)),IF(F11=0,1000000,F11*C11))=1000000,0,MIN(IF(I11=0,1000000,I11*ROUNDUP(C11,-3)),IF(H11=0,1000000,H11*ROUNDUP(C11,-2)),IF(G11=0,1000000,G11*ROUNDUP(C11,-1)),IF(F11=0,1000000,F11*C11)))</f>
         <v>0.5</v>
       </c>
       <c r="K11" s="2">
-        <f t="shared" si="5"/>
+        <f>IF(J11=IF(F11=0,1000000,F11*C11),C11,IF(J11=IF(G11=0,1000000,G11*ROUNDUP(C11,-1)),ROUNDUP(C11,-1),IF(J11=IF(H11=0,1000000,H11*ROUNDUP(C11,-2)),ROUNDUP(C11,-2),IF(J11=IF(I11=0,1000000,I11*ROUNDUP(C11,-3)),ROUNDUP(C11,-3),0))))</f>
         <v>1</v>
       </c>
       <c r="L11" t="s">
@@ -1543,10 +1562,10 @@
         <v>1</v>
       </c>
       <c r="C12" s="2">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D12" s="2" t="s">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>49</v>
       </c>
       <c r="E12" s="5" t="s">
@@ -1565,11 +1584,11 @@
         <v>1.54857</v>
       </c>
       <c r="J12" s="6">
-        <f t="shared" si="4"/>
+        <f>IF(MIN(IF(I12=0,1000000,I12*ROUNDUP(C12,-3)),IF(H12=0,1000000,H12*ROUNDUP(C12,-2)),IF(G12=0,1000000,G12*ROUNDUP(C12,-1)),IF(F12=0,1000000,F12*C12))=1000000,0,MIN(IF(I12=0,1000000,I12*ROUNDUP(C12,-3)),IF(H12=0,1000000,H12*ROUNDUP(C12,-2)),IF(G12=0,1000000,G12*ROUNDUP(C12,-1)),IF(F12=0,1000000,F12*C12)))</f>
         <v>2.52</v>
       </c>
       <c r="K12" s="2">
-        <f t="shared" si="5"/>
+        <f>IF(J12=IF(F12=0,1000000,F12*C12),C12,IF(J12=IF(G12=0,1000000,G12*ROUNDUP(C12,-1)),ROUNDUP(C12,-1),IF(J12=IF(H12=0,1000000,H12*ROUNDUP(C12,-2)),ROUNDUP(C12,-2),IF(J12=IF(I12=0,1000000,I12*ROUNDUP(C12,-3)),ROUNDUP(C12,-3),0))))</f>
         <v>1</v>
       </c>
       <c r="L12" s="2" t="s">
@@ -1581,7 +1600,7 @@
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
       <c r="AC12" s="2"/>
-      <c r="AD12" s="8"/>
+      <c r="AD12" s="11"/>
       <c r="AE12" s="5"/>
       <c r="AF12" s="2"/>
       <c r="AG12" s="2"/>
@@ -1601,45 +1620,45 @@
         <v>3</v>
       </c>
       <c r="C13" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D13" s="12">
-        <v>1</v>
+      <c r="D13" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="2">
+        <v>54</v>
+      </c>
+      <c r="F13">
         <v>0.10000000000000001</v>
       </c>
-      <c r="G13" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="H13" s="2">
-        <v>0.0091000000000000004</v>
-      </c>
-      <c r="I13" s="2">
-        <v>0.0047999999999999996</v>
+      <c r="G13">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="H13">
+        <v>0.0356</v>
+      </c>
+      <c r="I13">
+        <v>0.0223</v>
       </c>
       <c r="J13" s="6">
-        <f t="shared" si="4"/>
-        <v>0.20000000000000001</v>
+        <f>IF(MIN(IF(I13=0,1000000,I13*ROUNDUP(C13,-3)),IF(H13=0,1000000,H13*ROUNDUP(C13,-2)),IF(G13=0,1000000,G13*ROUNDUP(C13,-1)),IF(F13=0,1000000,F13*C13))=1000000,0,MIN(IF(I13=0,1000000,I13*ROUNDUP(C13,-3)),IF(H13=0,1000000,H13*ROUNDUP(C13,-2)),IF(G13=0,1000000,G13*ROUNDUP(C13,-1)),IF(F13=0,1000000,F13*C13)))</f>
+        <v>0.30000000000000004</v>
       </c>
       <c r="K13" s="2">
-        <f t="shared" si="5"/>
-        <v>10</v>
+        <f>IF(J13=IF(F13=0,1000000,F13*C13),C13,IF(J13=IF(G13=0,1000000,G13*ROUNDUP(C13,-1)),ROUNDUP(C13,-1),IF(J13=IF(H13=0,1000000,H13*ROUNDUP(C13,-2)),ROUNDUP(C13,-2),IF(J13=IF(I13=0,1000000,I13*ROUNDUP(C13,-3)),ROUNDUP(C13,-3),0))))</f>
+        <v>3</v>
       </c>
       <c r="L13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
-      <c r="R13" s="12"/>
+      <c r="R13" s="15"/>
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
       <c r="AC13" s="2"/>
-      <c r="AD13" s="13"/>
+      <c r="AD13" s="16"/>
       <c r="AE13" s="5"/>
       <c r="AF13" s="2"/>
       <c r="AG13" s="2"/>
@@ -1653,51 +1672,51 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B14" s="2">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C14" s="2">
-        <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="D14" s="14">
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D14" s="17">
+        <v>1</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F14" s="2">
         <v>0.10000000000000001</v>
       </c>
       <c r="G14" s="2">
-        <v>0.019</v>
+        <v>0.02</v>
       </c>
       <c r="H14" s="2">
-        <v>0.0086</v>
+        <v>0.0091000000000000004</v>
       </c>
       <c r="I14" s="2">
-        <v>0.0044799999999999996</v>
+        <v>0.0047999999999999996</v>
       </c>
       <c r="J14" s="6">
-        <f t="shared" si="4"/>
-        <v>0.38</v>
+        <f>IF(MIN(IF(I14=0,1000000,I14*ROUNDUP(C14,-3)),IF(H14=0,1000000,H14*ROUNDUP(C14,-2)),IF(G14=0,1000000,G14*ROUNDUP(C14,-1)),IF(F14=0,1000000,F14*C14))=1000000,0,MIN(IF(I14=0,1000000,I14*ROUNDUP(C14,-3)),IF(H14=0,1000000,H14*ROUNDUP(C14,-2)),IF(G14=0,1000000,G14*ROUNDUP(C14,-1)),IF(F14=0,1000000,F14*C14)))</f>
+        <v>0.20000000000000001</v>
       </c>
       <c r="K14" s="2">
-        <f t="shared" si="5"/>
-        <v>20</v>
+        <f>IF(J14=IF(F14=0,1000000,F14*C14),C14,IF(J14=IF(G14=0,1000000,G14*ROUNDUP(C14,-1)),ROUNDUP(C14,-1),IF(J14=IF(H14=0,1000000,H14*ROUNDUP(C14,-2)),ROUNDUP(C14,-2),IF(J14=IF(I14=0,1000000,I14*ROUNDUP(C14,-3)),ROUNDUP(C14,-3),0))))</f>
+        <v>10</v>
       </c>
       <c r="L14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
-      <c r="R14" s="14"/>
+      <c r="R14" s="18"/>
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
       <c r="AC14" s="2"/>
-      <c r="AD14" s="15"/>
+      <c r="AD14" s="19"/>
       <c r="AE14" s="5"/>
       <c r="AF14" s="2"/>
       <c r="AG14" s="2"/>
@@ -1711,51 +1730,51 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B15" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C15" s="2">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="D15" s="16">
-        <v>5.0999999999999996</v>
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="D15" s="20">
+        <v>10</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F15" s="2">
         <v>0.10000000000000001</v>
       </c>
       <c r="G15" s="2">
-        <v>0.089999999999999997</v>
+        <v>0.019</v>
       </c>
       <c r="H15" s="2">
-        <v>0.0082000000000000007</v>
+        <v>0.0086</v>
       </c>
       <c r="I15" s="2">
-        <v>0.0051000000000000004</v>
+        <v>0.0044799999999999996</v>
       </c>
       <c r="J15" s="6">
-        <f t="shared" si="4"/>
-        <v>0.70000000000000007</v>
+        <f>IF(MIN(IF(I15=0,1000000,I15*ROUNDUP(C15,-3)),IF(H15=0,1000000,H15*ROUNDUP(C15,-2)),IF(G15=0,1000000,G15*ROUNDUP(C15,-1)),IF(F15=0,1000000,F15*C15))=1000000,0,MIN(IF(I15=0,1000000,I15*ROUNDUP(C15,-3)),IF(H15=0,1000000,H15*ROUNDUP(C15,-2)),IF(G15=0,1000000,G15*ROUNDUP(C15,-1)),IF(F15=0,1000000,F15*C15)))</f>
+        <v>0.19</v>
       </c>
       <c r="K15" s="2">
-        <f t="shared" si="5"/>
-        <v>7</v>
+        <f>IF(J15=IF(F15=0,1000000,F15*C15),C15,IF(J15=IF(G15=0,1000000,G15*ROUNDUP(C15,-1)),ROUNDUP(C15,-1),IF(J15=IF(H15=0,1000000,H15*ROUNDUP(C15,-2)),ROUNDUP(C15,-2),IF(J15=IF(I15=0,1000000,I15*ROUNDUP(C15,-3)),ROUNDUP(C15,-3),0))))</f>
+        <v>10</v>
       </c>
       <c r="L15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
-      <c r="R15" s="16"/>
+      <c r="R15" s="21"/>
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
-      <c r="AD15" s="17"/>
+      <c r="AD15" s="22"/>
       <c r="AE15" s="5"/>
       <c r="AF15" s="2"/>
       <c r="AG15" s="2"/>
@@ -1769,43 +1788,43 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B16" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C16" s="2">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="D16" s="2">
-        <v>500</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="D16" s="23">
+        <v>5.0999999999999996</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F16" s="2">
         <v>0.10000000000000001</v>
       </c>
       <c r="G16" s="2">
-        <v>0.064000000000000001</v>
+        <v>0.089999999999999997</v>
       </c>
       <c r="H16" s="2">
-        <v>0.0533</v>
+        <v>0.0082000000000000007</v>
       </c>
       <c r="I16" s="2">
-        <v>0.044319999999999998</v>
+        <v>0.0051000000000000004</v>
       </c>
       <c r="J16" s="6">
-        <f t="shared" si="4"/>
-        <v>0.30000000000000004</v>
+        <f>IF(MIN(IF(I16=0,1000000,I16*ROUNDUP(C16,-3)),IF(H16=0,1000000,H16*ROUNDUP(C16,-2)),IF(G16=0,1000000,G16*ROUNDUP(C16,-1)),IF(F16=0,1000000,F16*C16))=1000000,0,MIN(IF(I16=0,1000000,I16*ROUNDUP(C16,-3)),IF(H16=0,1000000,H16*ROUNDUP(C16,-2)),IF(G16=0,1000000,G16*ROUNDUP(C16,-1)),IF(F16=0,1000000,F16*C16)))</f>
+        <v>0.70000000000000007</v>
       </c>
       <c r="K16" s="2">
-        <f t="shared" si="5"/>
-        <v>3</v>
+        <f>IF(J16=IF(F16=0,1000000,F16*C16),C16,IF(J16=IF(G16=0,1000000,G16*ROUNDUP(C16,-1)),ROUNDUP(C16,-1),IF(J16=IF(H16=0,1000000,H16*ROUNDUP(C16,-2)),ROUNDUP(C16,-2),IF(J16=IF(I16=0,1000000,I16*ROUNDUP(C16,-3)),ROUNDUP(C16,-3),0))))</f>
+        <v>7</v>
       </c>
       <c r="L16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
@@ -1813,7 +1832,7 @@
       <c r="AA16" s="2"/>
       <c r="AB16" s="2"/>
       <c r="AC16" s="2"/>
-      <c r="AD16" s="17"/>
+      <c r="AD16" s="22"/>
       <c r="AE16" s="5"/>
       <c r="AF16" s="2"/>
       <c r="AG16" s="2"/>
@@ -1827,51 +1846,51 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B17" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C17" s="2">
-        <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="D17" s="12">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
+      <c r="D17" s="10">
+        <v>500</v>
+      </c>
       <c r="E17" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F17" s="2">
         <v>0.10000000000000001</v>
       </c>
       <c r="G17" s="2">
-        <v>0.060999999999999999</v>
+        <v>0.064000000000000001</v>
       </c>
       <c r="H17" s="2">
-        <v>0.050599999999999999</v>
+        <v>0.0533</v>
       </c>
       <c r="I17" s="2">
-        <v>0.04206</v>
+        <v>0.044319999999999998</v>
       </c>
       <c r="J17" s="6">
-        <f t="shared" si="4"/>
-        <v>0.60000000000000009</v>
+        <f>IF(MIN(IF(I17=0,1000000,I17*ROUNDUP(C17,-3)),IF(H17=0,1000000,H17*ROUNDUP(C17,-2)),IF(G17=0,1000000,G17*ROUNDUP(C17,-1)),IF(F17=0,1000000,F17*C17))=1000000,0,MIN(IF(I17=0,1000000,I17*ROUNDUP(C17,-3)),IF(H17=0,1000000,H17*ROUNDUP(C17,-2)),IF(G17=0,1000000,G17*ROUNDUP(C17,-1)),IF(F17=0,1000000,F17*C17)))</f>
+        <v>0.30000000000000004</v>
       </c>
       <c r="K17" s="2">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="L17" s="18" t="s">
-        <v>66</v>
+        <f>IF(J17=IF(F17=0,1000000,F17*C17),C17,IF(J17=IF(G17=0,1000000,G17*ROUNDUP(C17,-1)),ROUNDUP(C17,-1),IF(J17=IF(H17=0,1000000,H17*ROUNDUP(C17,-2)),ROUNDUP(C17,-2),IF(J17=IF(I17=0,1000000,I17*ROUNDUP(C17,-3)),ROUNDUP(C17,-3),0))))</f>
+        <v>3</v>
+      </c>
+      <c r="L17" t="s">
+        <v>67</v>
       </c>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
-      <c r="R17" s="12"/>
+      <c r="R17" s="15"/>
       <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
       <c r="AC17" s="2"/>
-      <c r="AD17" s="13"/>
+      <c r="AD17" s="16"/>
       <c r="AE17" s="5"/>
       <c r="AF17" s="2"/>
       <c r="AG17" s="2"/>
@@ -1885,42 +1904,42 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B18" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C18" s="2">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>68</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D18" s="17">
+        <v>3</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>69</v>
       </c>
       <c r="F18" s="2">
-        <v>1.3799999999999999</v>
+        <v>0.10000000000000001</v>
       </c>
       <c r="G18" s="2">
-        <v>1.0069999999999999</v>
+        <v>0.060999999999999999</v>
       </c>
       <c r="H18" s="2">
-        <v>0.80930000000000002</v>
+        <v>0.050599999999999999</v>
       </c>
       <c r="I18" s="2">
-        <v>0.70565</v>
+        <v>0.04206</v>
       </c>
       <c r="J18" s="6">
-        <f t="shared" si="4"/>
-        <v>1.3799999999999999</v>
+        <f>IF(MIN(IF(I18=0,1000000,I18*ROUNDUP(C18,-3)),IF(H18=0,1000000,H18*ROUNDUP(C18,-2)),IF(G18=0,1000000,G18*ROUNDUP(C18,-1)),IF(F18=0,1000000,F18*C18))=1000000,0,MIN(IF(I18=0,1000000,I18*ROUNDUP(C18,-3)),IF(H18=0,1000000,H18*ROUNDUP(C18,-2)),IF(G18=0,1000000,G18*ROUNDUP(C18,-1)),IF(F18=0,1000000,F18*C18)))</f>
+        <v>0.30000000000000004</v>
       </c>
       <c r="K18" s="2">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="L18" t="s">
+        <f>IF(J18=IF(F18=0,1000000,F18*C18),C18,IF(J18=IF(G18=0,1000000,G18*ROUNDUP(C18,-1)),ROUNDUP(C18,-1),IF(J18=IF(H18=0,1000000,H18*ROUNDUP(C18,-2)),ROUNDUP(C18,-2),IF(J18=IF(I18=0,1000000,I18*ROUNDUP(C18,-3)),ROUNDUP(C18,-3),0))))</f>
+        <v>3</v>
+      </c>
+      <c r="L18" s="24" t="s">
         <v>70</v>
       </c>
       <c r="P18" s="2"/>
@@ -1949,33 +1968,33 @@
         <v>1</v>
       </c>
       <c r="C19" s="2">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D19" s="2" t="s">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>72</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>73</v>
       </c>
       <c r="F19" s="2">
-        <v>1.53</v>
+        <v>1.3799999999999999</v>
       </c>
       <c r="G19" s="2">
-        <v>1.431</v>
+        <v>1.0069999999999999</v>
       </c>
       <c r="H19" s="2">
-        <v>1.3285</v>
+        <v>0.80930000000000002</v>
       </c>
       <c r="I19" s="2">
-        <v>1.2256800000000001</v>
+        <v>0.70565</v>
       </c>
       <c r="J19" s="6">
-        <f t="shared" si="4"/>
-        <v>1.53</v>
+        <f>IF(MIN(IF(I19=0,1000000,I19*ROUNDUP(C19,-3)),IF(H19=0,1000000,H19*ROUNDUP(C19,-2)),IF(G19=0,1000000,G19*ROUNDUP(C19,-1)),IF(F19=0,1000000,F19*C19))=1000000,0,MIN(IF(I19=0,1000000,I19*ROUNDUP(C19,-3)),IF(H19=0,1000000,H19*ROUNDUP(C19,-2)),IF(G19=0,1000000,G19*ROUNDUP(C19,-1)),IF(F19=0,1000000,F19*C19)))</f>
+        <v>1.3799999999999999</v>
       </c>
       <c r="K19" s="2">
-        <f t="shared" si="5"/>
+        <f>IF(J19=IF(F19=0,1000000,F19*C19),C19,IF(J19=IF(G19=0,1000000,G19*ROUNDUP(C19,-1)),ROUNDUP(C19,-1),IF(J19=IF(H19=0,1000000,H19*ROUNDUP(C19,-2)),ROUNDUP(C19,-2),IF(J19=IF(I19=0,1000000,I19*ROUNDUP(C19,-3)),ROUNDUP(C19,-3),0))))</f>
         <v>1</v>
       </c>
       <c r="L19" t="s">
@@ -1987,7 +2006,7 @@
       <c r="AA19" s="2"/>
       <c r="AB19" s="2"/>
       <c r="AC19" s="2"/>
-      <c r="AD19" s="19"/>
+      <c r="AD19" s="25"/>
       <c r="AE19" s="5"/>
       <c r="AF19" s="2"/>
       <c r="AG19" s="2"/>
@@ -2007,29 +2026,33 @@
         <v>1</v>
       </c>
       <c r="C20" s="2">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D20" s="2" t="s">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>76</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>77</v>
       </c>
       <c r="F20" s="2">
-        <v>8.6099999999999994</v>
+        <v>1.53</v>
       </c>
       <c r="G20" s="2">
-        <v>6.6849999999999996</v>
-      </c>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
+        <v>1.431</v>
+      </c>
+      <c r="H20" s="2">
+        <v>1.3285</v>
+      </c>
+      <c r="I20" s="2">
+        <v>1.2256800000000001</v>
+      </c>
       <c r="J20" s="6">
-        <f t="shared" si="4"/>
-        <v>8.6099999999999994</v>
+        <f>IF(MIN(IF(I20=0,1000000,I20*ROUNDUP(C20,-3)),IF(H20=0,1000000,H20*ROUNDUP(C20,-2)),IF(G20=0,1000000,G20*ROUNDUP(C20,-1)),IF(F20=0,1000000,F20*C20))=1000000,0,MIN(IF(I20=0,1000000,I20*ROUNDUP(C20,-3)),IF(H20=0,1000000,H20*ROUNDUP(C20,-2)),IF(G20=0,1000000,G20*ROUNDUP(C20,-1)),IF(F20=0,1000000,F20*C20)))</f>
+        <v>1.53</v>
       </c>
       <c r="K20" s="2">
-        <f t="shared" si="5"/>
+        <f>IF(J20=IF(F20=0,1000000,F20*C20),C20,IF(J20=IF(G20=0,1000000,G20*ROUNDUP(C20,-1)),ROUNDUP(C20,-1),IF(J20=IF(H20=0,1000000,H20*ROUNDUP(C20,-2)),ROUNDUP(C20,-2),IF(J20=IF(I20=0,1000000,I20*ROUNDUP(C20,-3)),ROUNDUP(C20,-3),0))))</f>
         <v>1</v>
       </c>
       <c r="L20" t="s">
@@ -2061,33 +2084,29 @@
         <v>1</v>
       </c>
       <c r="C21" s="2">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D21" s="2" t="s">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D21" s="10" t="s">
         <v>80</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F21" s="2">
-        <v>0.95999999999999996</v>
+        <v>8.6099999999999994</v>
       </c>
       <c r="G21" s="2">
-        <v>0.81000000000000005</v>
-      </c>
-      <c r="H21" s="2">
-        <v>0.68359999999999999</v>
-      </c>
-      <c r="I21" s="2">
-        <v>0.59601000000000004</v>
-      </c>
+        <v>6.6849999999999996</v>
+      </c>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
       <c r="J21" s="6">
-        <f t="shared" si="4"/>
-        <v>0.95999999999999996</v>
+        <f>IF(MIN(IF(I21=0,1000000,I21*ROUNDUP(C21,-3)),IF(H21=0,1000000,H21*ROUNDUP(C21,-2)),IF(G21=0,1000000,G21*ROUNDUP(C21,-1)),IF(F21=0,1000000,F21*C21))=1000000,0,MIN(IF(I21=0,1000000,I21*ROUNDUP(C21,-3)),IF(H21=0,1000000,H21*ROUNDUP(C21,-2)),IF(G21=0,1000000,G21*ROUNDUP(C21,-1)),IF(F21=0,1000000,F21*C21)))</f>
+        <v>8.6099999999999994</v>
       </c>
       <c r="K21" s="2">
-        <f t="shared" si="5"/>
+        <f>IF(J21=IF(F21=0,1000000,F21*C21),C21,IF(J21=IF(G21=0,1000000,G21*ROUNDUP(C21,-1)),ROUNDUP(C21,-1),IF(J21=IF(H21=0,1000000,H21*ROUNDUP(C21,-2)),ROUNDUP(C21,-2),IF(J21=IF(I21=0,1000000,I21*ROUNDUP(C21,-3)),ROUNDUP(C21,-3),0))))</f>
         <v>1</v>
       </c>
       <c r="L21" t="s">
@@ -2107,7 +2126,7 @@
       <c r="AI21" s="2"/>
       <c r="AJ21" s="6"/>
       <c r="AK21" s="2"/>
-      <c r="AL21" s="18"/>
+      <c r="AL21" s="24"/>
       <c r="AM21" s="2"/>
       <c r="AN21" s="2"/>
     </row>
@@ -2119,33 +2138,33 @@
         <v>1</v>
       </c>
       <c r="C22" s="2">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D22" s="2" t="s">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D22" s="10" t="s">
         <v>84</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>85</v>
       </c>
       <c r="F22" s="2">
-        <v>7.2599999999999998</v>
+        <v>0.95999999999999996</v>
       </c>
       <c r="G22" s="2">
-        <v>6.282</v>
+        <v>0.81000000000000005</v>
       </c>
       <c r="H22" s="2">
-        <v>5.9656000000000002</v>
+        <v>0.68359999999999999</v>
       </c>
       <c r="I22" s="2">
-        <v>5.5507999999999997</v>
+        <v>0.59601000000000004</v>
       </c>
       <c r="J22" s="6">
-        <f t="shared" si="4"/>
-        <v>7.2599999999999998</v>
+        <f>IF(MIN(IF(I22=0,1000000,I22*ROUNDUP(C22,-3)),IF(H22=0,1000000,H22*ROUNDUP(C22,-2)),IF(G22=0,1000000,G22*ROUNDUP(C22,-1)),IF(F22=0,1000000,F22*C22))=1000000,0,MIN(IF(I22=0,1000000,I22*ROUNDUP(C22,-3)),IF(H22=0,1000000,H22*ROUNDUP(C22,-2)),IF(G22=0,1000000,G22*ROUNDUP(C22,-1)),IF(F22=0,1000000,F22*C22)))</f>
+        <v>0.95999999999999996</v>
       </c>
       <c r="K22" s="2">
-        <f t="shared" si="5"/>
+        <f>IF(J22=IF(F22=0,1000000,F22*C22),C22,IF(J22=IF(G22=0,1000000,G22*ROUNDUP(C22,-1)),ROUNDUP(C22,-1),IF(J22=IF(H22=0,1000000,H22*ROUNDUP(C22,-2)),ROUNDUP(C22,-2),IF(J22=IF(I22=0,1000000,I22*ROUNDUP(C22,-3)),ROUNDUP(C22,-3),0))))</f>
         <v>1</v>
       </c>
       <c r="L22" t="s">
@@ -2177,33 +2196,33 @@
         <v>1</v>
       </c>
       <c r="C23" s="2">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D23" s="2" t="s">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D23" s="10" t="s">
         <v>88</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>89</v>
       </c>
       <c r="F23" s="2">
-        <v>8.7200000000000006</v>
+        <v>7.2599999999999998</v>
       </c>
       <c r="G23" s="2">
-        <v>7.5700000000000003</v>
+        <v>6.282</v>
       </c>
       <c r="H23" s="2">
-        <v>6.7085999999999997</v>
+        <v>5.9656000000000002</v>
       </c>
       <c r="I23" s="2">
-        <v>6.0628700000000002</v>
+        <v>5.5507999999999997</v>
       </c>
       <c r="J23" s="6">
-        <f t="shared" si="4"/>
-        <v>8.7200000000000006</v>
+        <f>IF(MIN(IF(I23=0,1000000,I23*ROUNDUP(C23,-3)),IF(H23=0,1000000,H23*ROUNDUP(C23,-2)),IF(G23=0,1000000,G23*ROUNDUP(C23,-1)),IF(F23=0,1000000,F23*C23))=1000000,0,MIN(IF(I23=0,1000000,I23*ROUNDUP(C23,-3)),IF(H23=0,1000000,H23*ROUNDUP(C23,-2)),IF(G23=0,1000000,G23*ROUNDUP(C23,-1)),IF(F23=0,1000000,F23*C23)))</f>
+        <v>7.2599999999999998</v>
       </c>
       <c r="K23" s="2">
-        <f t="shared" si="5"/>
+        <f>IF(J23=IF(F23=0,1000000,F23*C23),C23,IF(J23=IF(G23=0,1000000,G23*ROUNDUP(C23,-1)),ROUNDUP(C23,-1),IF(J23=IF(H23=0,1000000,H23*ROUNDUP(C23,-2)),ROUNDUP(C23,-2),IF(J23=IF(I23=0,1000000,I23*ROUNDUP(C23,-3)),ROUNDUP(C23,-3),0))))</f>
         <v>1</v>
       </c>
       <c r="L23" t="s">
@@ -2215,7 +2234,7 @@
       <c r="AA23" s="2"/>
       <c r="AB23" s="2"/>
       <c r="AC23" s="2"/>
-      <c r="AD23" s="10"/>
+      <c r="AD23" s="13"/>
       <c r="AE23" s="5"/>
       <c r="AF23" s="2"/>
       <c r="AG23" s="2"/>
@@ -2235,31 +2254,33 @@
         <v>1</v>
       </c>
       <c r="C24" s="2">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D24" s="2" t="s">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D24" s="10" t="s">
         <v>92</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>93</v>
       </c>
       <c r="F24" s="2">
-        <v>31.5</v>
+        <v>8.7200000000000006</v>
       </c>
       <c r="G24" s="2">
-        <v>25.91</v>
+        <v>7.5700000000000003</v>
       </c>
       <c r="H24" s="2">
-        <v>20.853899999999999</v>
-      </c>
-      <c r="I24" s="2"/>
+        <v>6.7085999999999997</v>
+      </c>
+      <c r="I24" s="2">
+        <v>6.0628700000000002</v>
+      </c>
       <c r="J24" s="6">
-        <f t="shared" si="4"/>
-        <v>31.5</v>
+        <f>IF(MIN(IF(I24=0,1000000,I24*ROUNDUP(C24,-3)),IF(H24=0,1000000,H24*ROUNDUP(C24,-2)),IF(G24=0,1000000,G24*ROUNDUP(C24,-1)),IF(F24=0,1000000,F24*C24))=1000000,0,MIN(IF(I24=0,1000000,I24*ROUNDUP(C24,-3)),IF(H24=0,1000000,H24*ROUNDUP(C24,-2)),IF(G24=0,1000000,G24*ROUNDUP(C24,-1)),IF(F24=0,1000000,F24*C24)))</f>
+        <v>8.7200000000000006</v>
       </c>
       <c r="K24" s="2">
-        <f t="shared" si="5"/>
+        <f>IF(J24=IF(F24=0,1000000,F24*C24),C24,IF(J24=IF(G24=0,1000000,G24*ROUNDUP(C24,-1)),ROUNDUP(C24,-1),IF(J24=IF(H24=0,1000000,H24*ROUNDUP(C24,-2)),ROUNDUP(C24,-2),IF(J24=IF(I24=0,1000000,I24*ROUNDUP(C24,-3)),ROUNDUP(C24,-3),0))))</f>
         <v>1</v>
       </c>
       <c r="L24" t="s">
@@ -2291,24 +2312,31 @@
         <v>1</v>
       </c>
       <c r="C25" s="2">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D25" s="2" t="s">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D25" s="10" t="s">
         <v>96</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F25">
-        <v>8.1199999999999992</v>
-      </c>
+      <c r="F25" s="2">
+        <v>31.5</v>
+      </c>
+      <c r="G25" s="2">
+        <v>25.91</v>
+      </c>
+      <c r="H25" s="2">
+        <v>20.853899999999999</v>
+      </c>
+      <c r="I25" s="2"/>
       <c r="J25" s="6">
-        <f t="shared" si="4"/>
-        <v>8.1199999999999992</v>
+        <f>IF(MIN(IF(I25=0,1000000,I25*ROUNDUP(C25,-3)),IF(H25=0,1000000,H25*ROUNDUP(C25,-2)),IF(G25=0,1000000,G25*ROUNDUP(C25,-1)),IF(F25=0,1000000,F25*C25))=1000000,0,MIN(IF(I25=0,1000000,I25*ROUNDUP(C25,-3)),IF(H25=0,1000000,H25*ROUNDUP(C25,-2)),IF(G25=0,1000000,G25*ROUNDUP(C25,-1)),IF(F25=0,1000000,F25*C25)))</f>
+        <v>31.5</v>
       </c>
       <c r="K25" s="2">
-        <f t="shared" si="5"/>
+        <f>IF(J25=IF(F25=0,1000000,F25*C25),C25,IF(J25=IF(G25=0,1000000,G25*ROUNDUP(C25,-1)),ROUNDUP(C25,-1),IF(J25=IF(H25=0,1000000,H25*ROUNDUP(C25,-2)),ROUNDUP(C25,-2),IF(J25=IF(I25=0,1000000,I25*ROUNDUP(C25,-3)),ROUNDUP(C25,-3),0))))</f>
         <v>1</v>
       </c>
       <c r="L25" t="s">
@@ -2320,7 +2348,7 @@
       <c r="AA25" s="2"/>
       <c r="AB25" s="2"/>
       <c r="AC25" s="2"/>
-      <c r="AD25" s="20"/>
+      <c r="AD25" s="26"/>
       <c r="AE25" s="5"/>
       <c r="AF25" s="2"/>
       <c r="AG25" s="2"/>
@@ -2337,37 +2365,28 @@
         <v>99</v>
       </c>
       <c r="B26" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C26" s="2">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="D26" s="2" t="s">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D26" s="10" t="s">
         <v>100</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="F26" s="2">
-        <v>0.46999999999999997</v>
-      </c>
-      <c r="G26" s="2">
-        <v>0.32900000000000001</v>
-      </c>
-      <c r="H26" s="2">
-        <v>0.25490000000000002</v>
-      </c>
-      <c r="I26" s="2">
-        <v>0.21598999999999999</v>
+      <c r="F26">
+        <v>8.1199999999999992</v>
       </c>
       <c r="J26" s="6">
-        <f t="shared" si="4"/>
-        <v>1.4099999999999999</v>
+        <f>IF(MIN(IF(I26=0,1000000,I26*ROUNDUP(C26,-3)),IF(H26=0,1000000,H26*ROUNDUP(C26,-2)),IF(G26=0,1000000,G26*ROUNDUP(C26,-1)),IF(F26=0,1000000,F26*C26))=1000000,0,MIN(IF(I26=0,1000000,I26*ROUNDUP(C26,-3)),IF(H26=0,1000000,H26*ROUNDUP(C26,-2)),IF(G26=0,1000000,G26*ROUNDUP(C26,-1)),IF(F26=0,1000000,F26*C26)))</f>
+        <v>8.1199999999999992</v>
       </c>
       <c r="K26" s="2">
-        <f t="shared" si="5"/>
-        <v>3</v>
+        <f>IF(J26=IF(F26=0,1000000,F26*C26),C26,IF(J26=IF(G26=0,1000000,G26*ROUNDUP(C26,-1)),ROUNDUP(C26,-1),IF(J26=IF(H26=0,1000000,H26*ROUNDUP(C26,-2)),ROUNDUP(C26,-2),IF(J26=IF(I26=0,1000000,I26*ROUNDUP(C26,-3)),ROUNDUP(C26,-3),0))))</f>
+        <v>1</v>
       </c>
       <c r="L26" t="s">
         <v>102</v>
@@ -2378,7 +2397,7 @@
       <c r="AA26" s="2"/>
       <c r="AB26" s="2"/>
       <c r="AC26" s="2"/>
-      <c r="AD26" s="20"/>
+      <c r="AD26" s="26"/>
       <c r="AE26" s="5"/>
       <c r="AF26" s="2"/>
       <c r="AG26" s="2"/>
@@ -2398,10 +2417,10 @@
         <v>1</v>
       </c>
       <c r="C27" s="2">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D27" s="2" t="s">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D27" s="10" t="s">
         <v>104</v>
       </c>
       <c r="E27" s="5" t="s">
@@ -2420,11 +2439,11 @@
         <v>0.15112999999999999</v>
       </c>
       <c r="J27" s="6">
-        <f t="shared" si="4"/>
+        <f>IF(MIN(IF(I27=0,1000000,I27*ROUNDUP(C27,-3)),IF(H27=0,1000000,H27*ROUNDUP(C27,-2)),IF(G27=0,1000000,G27*ROUNDUP(C27,-1)),IF(F27=0,1000000,F27*C27))=1000000,0,MIN(IF(I27=0,1000000,I27*ROUNDUP(C27,-3)),IF(H27=0,1000000,H27*ROUNDUP(C27,-2)),IF(G27=0,1000000,G27*ROUNDUP(C27,-1)),IF(F27=0,1000000,F27*C27)))</f>
         <v>0.23000000000000001</v>
       </c>
       <c r="K27" s="2">
-        <f t="shared" si="5"/>
+        <f>IF(J27=IF(F27=0,1000000,F27*C27),C27,IF(J27=IF(G27=0,1000000,G27*ROUNDUP(C27,-1)),ROUNDUP(C27,-1),IF(J27=IF(H27=0,1000000,H27*ROUNDUP(C27,-2)),ROUNDUP(C27,-2),IF(J27=IF(I27=0,1000000,I27*ROUNDUP(C27,-3)),ROUNDUP(C27,-3),0))))</f>
         <v>1</v>
       </c>
       <c r="L27" t="s">
@@ -2436,7 +2455,7 @@
       <c r="AA27" s="2"/>
       <c r="AB27" s="2"/>
       <c r="AC27" s="2"/>
-      <c r="AD27" s="21"/>
+      <c r="AD27" s="27"/>
       <c r="AE27" s="5"/>
       <c r="AF27" s="2"/>
       <c r="AG27" s="2"/>
@@ -2456,10 +2475,10 @@
         <v>1</v>
       </c>
       <c r="C28" s="2">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D28" s="2" t="s">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D28" s="10" t="s">
         <v>107</v>
       </c>
       <c r="E28" s="2" t="s">
@@ -2473,11 +2492,11 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="6">
-        <f t="shared" si="4"/>
+        <f>IF(MIN(IF(I28=0,1000000,I28*ROUNDUP(C28,-3)),IF(H28=0,1000000,H28*ROUNDUP(C28,-2)),IF(G28=0,1000000,G28*ROUNDUP(C28,-1)),IF(F28=0,1000000,F28*C28))=1000000,0,MIN(IF(I28=0,1000000,I28*ROUNDUP(C28,-3)),IF(H28=0,1000000,H28*ROUNDUP(C28,-2)),IF(G28=0,1000000,G28*ROUNDUP(C28,-1)),IF(F28=0,1000000,F28*C28)))</f>
         <v>13.950000000000001</v>
       </c>
       <c r="K28" s="2">
-        <f t="shared" si="5"/>
+        <f>IF(J28=IF(F28=0,1000000,F28*C28),C28,IF(J28=IF(G28=0,1000000,G28*ROUNDUP(C28,-1)),ROUNDUP(C28,-1),IF(J28=IF(H28=0,1000000,H28*ROUNDUP(C28,-2)),ROUNDUP(C28,-2),IF(J28=IF(I28=0,1000000,I28*ROUNDUP(C28,-3)),ROUNDUP(C28,-3),0))))</f>
         <v>1</v>
       </c>
       <c r="P28" s="2"/>
@@ -2486,7 +2505,7 @@
       <c r="AA28" s="2"/>
       <c r="AB28" s="2"/>
       <c r="AC28" s="2"/>
-      <c r="AD28" s="10"/>
+      <c r="AD28" s="13"/>
       <c r="AE28" s="5"/>
       <c r="AF28" s="2"/>
       <c r="AG28" s="2"/>
@@ -2505,7 +2524,7 @@
       <c r="AA29" s="2"/>
       <c r="AB29" s="2"/>
       <c r="AC29" s="2"/>
-      <c r="AD29" s="12"/>
+      <c r="AD29" s="15"/>
       <c r="AE29" s="5"/>
       <c r="AF29" s="2"/>
       <c r="AG29" s="2"/>
@@ -2540,7 +2559,7 @@
       <c r="AA31" s="2"/>
       <c r="AB31" s="2"/>
       <c r="AC31" s="2"/>
-      <c r="AD31" s="14"/>
+      <c r="AD31" s="18"/>
       <c r="AE31" s="5"/>
       <c r="AF31" s="2"/>
       <c r="AG31" s="2"/>
@@ -2555,7 +2574,7 @@
     <row r="32">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
-      <c r="D32" s="12"/>
+      <c r="D32" s="15"/>
       <c r="E32" s="5"/>
       <c r="J32" s="6"/>
       <c r="K32" s="2"/>
@@ -2580,7 +2599,7 @@
       <c r="AA33" s="2"/>
       <c r="AB33" s="2"/>
       <c r="AC33" s="2"/>
-      <c r="AD33" s="12"/>
+      <c r="AD33" s="15"/>
       <c r="AE33" s="5"/>
       <c r="AF33" s="2"/>
       <c r="AG33" s="2"/>
@@ -2595,14 +2614,14 @@
     <row r="34">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
-      <c r="D34" s="12"/>
+      <c r="D34" s="15"/>
       <c r="E34" s="5"/>
       <c r="J34" s="6"/>
       <c r="K34" s="2"/>
       <c r="AA34" s="2"/>
       <c r="AB34" s="2"/>
       <c r="AC34" s="2"/>
-      <c r="AD34" s="12"/>
+      <c r="AD34" s="15"/>
       <c r="AE34" s="5"/>
       <c r="AF34" s="2"/>
       <c r="AG34" s="2"/>
@@ -2625,9 +2644,9 @@
       <c r="I35" s="1"/>
       <c r="J35" s="6">
         <f>SUM(J3:J32)</f>
-        <v>94.27000000000001</v>
-      </c>
-      <c r="K35" s="22"/>
+        <v>92.670000000000016</v>
+      </c>
+      <c r="K35" s="28"/>
       <c r="AA35" s="2"/>
       <c r="AB35" s="2"/>
       <c r="AC35" s="2"/>
@@ -2646,7 +2665,7 @@
     <row r="36">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
-      <c r="D36" s="16"/>
+      <c r="D36" s="21"/>
       <c r="E36" s="5"/>
       <c r="H36" s="1" t="s">
         <v>110</v>
@@ -2654,12 +2673,12 @@
       <c r="I36" s="1"/>
       <c r="J36">
         <f>SUM(K3:K32)</f>
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="AA36" s="2"/>
       <c r="AB36" s="2"/>
       <c r="AC36" s="2"/>
-      <c r="AD36" s="16"/>
+      <c r="AD36" s="21"/>
       <c r="AE36" s="5"/>
       <c r="AF36" s="2"/>
       <c r="AG36" s="2"/>
@@ -2702,7 +2721,7 @@
       <c r="I38" s="1"/>
       <c r="J38" s="6">
         <f>J35/C1</f>
-        <v>94.27000000000001</v>
+        <v>92.670000000000016</v>
       </c>
       <c r="AA38" s="2"/>
       <c r="AB38" s="2"/>
@@ -2730,7 +2749,7 @@
       <c r="I39" s="1"/>
       <c r="J39">
         <f>J36/C1</f>
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="AA39" s="2"/>
       <c r="AB39" s="2"/>
@@ -2777,9 +2796,9 @@
         <v>113</v>
       </c>
       <c r="I41" s="1"/>
-      <c r="J41" s="23">
+      <c r="J41" s="29">
         <f>SUM(B3:B28)</f>
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="AA41" s="2"/>
       <c r="AB41" s="2"/>
@@ -2805,9 +2824,9 @@
         <v>114</v>
       </c>
       <c r="I42" s="1"/>
-      <c r="J42" s="24">
+      <c r="J42" s="30">
         <f>J41/J39</f>
-        <v>0.65420560747663548</v>
+        <v>0.64893617021276595</v>
       </c>
       <c r="AA42" s="2"/>
       <c r="AB42" s="2"/>
@@ -2932,12 +2951,12 @@
     <row r="48">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
-      <c r="D48" s="25"/>
+      <c r="D48" s="31"/>
       <c r="J48" s="6"/>
       <c r="AA48" s="2"/>
       <c r="AB48" s="2"/>
       <c r="AC48" s="2"/>
-      <c r="AD48" s="25"/>
+      <c r="AD48" s="31"/>
       <c r="AE48" s="2"/>
       <c r="AF48" s="2"/>
       <c r="AG48" s="2"/>
@@ -3039,7 +3058,7 @@
       <c r="AH53" s="1"/>
       <c r="AI53" s="1"/>
       <c r="AJ53" s="6"/>
-      <c r="AK53" s="22"/>
+      <c r="AK53" s="28"/>
       <c r="AL53" s="2"/>
       <c r="AM53" s="2"/>
       <c r="AN53" s="2"/>
@@ -3066,11 +3085,11 @@
     <row r="55">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
-      <c r="D55" s="25"/>
+      <c r="D55" s="31"/>
       <c r="AA55" s="2"/>
       <c r="AB55" s="2"/>
       <c r="AC55" s="2"/>
-      <c r="AD55" s="25"/>
+      <c r="AD55" s="31"/>
       <c r="AE55" s="2"/>
       <c r="AF55" s="2"/>
       <c r="AG55" s="2"/>

</xml_diff>